<commit_message>
Update Module 5 Challenge - Solved version (Excel Skills for Business: Essentials)
</commit_message>
<xml_diff>
--- a/C1-Essentials/Module 5 - Printing/Challenge/W05-Challenge-Solved.xlsx
+++ b/C1-Essentials/Module 5 - Printing/Challenge/W05-Challenge-Solved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurma\OneDrive\Documents\Data Analyst\Excel\Excel Skills for Business by Macquarie University\C1-Essentials\Module 5 - Printing\Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67CEF15F-BE6F-4791-ABA8-1E832B6BE68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37A12FA-00F9-4DAE-A118-8FFFB1813205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1252,7 +1252,7 @@
   </sheetPr>
   <dimension ref="A1:M1785"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -1350,7 +1350,7 @@
         <v>42371</v>
       </c>
       <c r="G4" s="8">
-        <f>F4-E4</f>
+        <f t="shared" ref="G4:G35" si="0">F4-E4</f>
         <v>10</v>
       </c>
       <c r="H4" s="2">
@@ -1360,18 +1360,18 @@
         <v>12.99</v>
       </c>
       <c r="J4" s="9">
-        <f>H4*I4</f>
+        <f t="shared" ref="J4:J35" si="1">H4*I4</f>
         <v>181.86</v>
       </c>
       <c r="K4" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L4" s="9">
-        <f>J4*K4</f>
+        <f t="shared" ref="L4:L35" si="2">J4*K4</f>
         <v>12.730200000000002</v>
       </c>
       <c r="M4" s="9">
-        <f>J4-L4</f>
+        <f t="shared" ref="M4:M35" si="3">J4-L4</f>
         <v>169.12980000000002</v>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
         <v>42371</v>
       </c>
       <c r="G5" s="8">
-        <f>F5-E5</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H5" s="2">
@@ -1405,18 +1405,18 @@
         <v>23.99</v>
       </c>
       <c r="J5" s="9">
-        <f>H5*I5</f>
+        <f t="shared" si="1"/>
         <v>407.83</v>
       </c>
       <c r="K5" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L5" s="9">
-        <f>J5*K5</f>
+        <f t="shared" si="2"/>
         <v>30.587249999999997</v>
       </c>
       <c r="M5" s="9">
-        <f>J5-L5</f>
+        <f t="shared" si="3"/>
         <v>377.24275</v>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
         <v>42381</v>
       </c>
       <c r="G6" s="8">
-        <f>F6-E6</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H6" s="2">
@@ -1450,18 +1450,18 @@
         <v>25.99</v>
       </c>
       <c r="J6" s="9">
-        <f>H6*I6</f>
+        <f t="shared" si="1"/>
         <v>389.84999999999997</v>
       </c>
       <c r="K6" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L6" s="9">
-        <f>J6*K6</f>
+        <f t="shared" si="2"/>
         <v>25.340249999999997</v>
       </c>
       <c r="M6" s="9">
-        <f>J6-L6</f>
+        <f t="shared" si="3"/>
         <v>364.50974999999994</v>
       </c>
     </row>
@@ -1485,7 +1485,7 @@
         <v>42384</v>
       </c>
       <c r="G7" s="8">
-        <f>F7-E7</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H7" s="2">
@@ -1495,18 +1495,18 @@
         <v>42.99</v>
       </c>
       <c r="J7" s="9">
-        <f>H7*I7</f>
+        <f t="shared" si="1"/>
         <v>1031.76</v>
       </c>
       <c r="K7" s="10">
         <v>0.06</v>
       </c>
       <c r="L7" s="9">
-        <f>J7*K7</f>
+        <f t="shared" si="2"/>
         <v>61.9056</v>
       </c>
       <c r="M7" s="9">
-        <f>J7-L7</f>
+        <f t="shared" si="3"/>
         <v>969.85439999999994</v>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
         <v>42414</v>
       </c>
       <c r="G8" s="8">
-        <f>F8-E8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H8" s="2">
@@ -1540,18 +1540,18 @@
         <v>37.99</v>
       </c>
       <c r="J8" s="9">
-        <f>H8*I8</f>
+        <f t="shared" si="1"/>
         <v>987.74</v>
       </c>
       <c r="K8" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L8" s="9">
-        <f>J8*K8</f>
+        <f t="shared" si="2"/>
         <v>69.141800000000003</v>
       </c>
       <c r="M8" s="9">
-        <f>J8-L8</f>
+        <f t="shared" si="3"/>
         <v>918.59820000000002</v>
       </c>
     </row>
@@ -1575,7 +1575,7 @@
         <v>42414</v>
       </c>
       <c r="G9" s="8">
-        <f>F9-E9</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="H9" s="2">
@@ -1585,18 +1585,18 @@
         <v>25.99</v>
       </c>
       <c r="J9" s="9">
-        <f>H9*I9</f>
+        <f t="shared" si="1"/>
         <v>623.76</v>
       </c>
       <c r="K9" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L9" s="9">
-        <f>J9*K9</f>
+        <f t="shared" si="2"/>
         <v>46.781999999999996</v>
       </c>
       <c r="M9" s="9">
-        <f>J9-L9</f>
+        <f t="shared" si="3"/>
         <v>576.97799999999995</v>
       </c>
     </row>
@@ -1620,7 +1620,7 @@
         <v>42422</v>
       </c>
       <c r="G10" s="8">
-        <f>F10-E10</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H10" s="2">
@@ -1630,18 +1630,18 @@
         <v>37.99</v>
       </c>
       <c r="J10" s="9">
-        <f>H10*I10</f>
+        <f t="shared" si="1"/>
         <v>987.74</v>
       </c>
       <c r="K10" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L10" s="9">
-        <f>J10*K10</f>
+        <f t="shared" si="2"/>
         <v>74.080500000000001</v>
       </c>
       <c r="M10" s="9">
-        <f>J10-L10</f>
+        <f t="shared" si="3"/>
         <v>913.65949999999998</v>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
         <v>42469</v>
       </c>
       <c r="G11" s="8">
-        <f>F11-E11</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H11" s="2">
@@ -1675,18 +1675,18 @@
         <v>23.99</v>
       </c>
       <c r="J11" s="9">
-        <f>H11*I11</f>
+        <f t="shared" si="1"/>
         <v>407.83</v>
       </c>
       <c r="K11" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L11" s="9">
-        <f>J11*K11</f>
+        <f t="shared" si="2"/>
         <v>30.587249999999997</v>
       </c>
       <c r="M11" s="9">
-        <f>J11-L11</f>
+        <f t="shared" si="3"/>
         <v>377.24275</v>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
         <v>42475</v>
       </c>
       <c r="G12" s="8">
-        <f>F12-E12</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H12" s="2">
@@ -1720,18 +1720,18 @@
         <v>25.99</v>
       </c>
       <c r="J12" s="9">
-        <f>H12*I12</f>
+        <f t="shared" si="1"/>
         <v>441.83</v>
       </c>
       <c r="K12" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L12" s="9">
-        <f>J12*K12</f>
+        <f t="shared" si="2"/>
         <v>33.137249999999995</v>
       </c>
       <c r="M12" s="9">
-        <f>J12-L12</f>
+        <f t="shared" si="3"/>
         <v>408.69274999999999</v>
       </c>
     </row>
@@ -1755,7 +1755,7 @@
         <v>42481</v>
       </c>
       <c r="G13" s="8">
-        <f>F13-E13</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H13" s="2">
@@ -1765,18 +1765,18 @@
         <v>42.99</v>
       </c>
       <c r="J13" s="9">
-        <f>H13*I13</f>
+        <f t="shared" si="1"/>
         <v>1117.74</v>
       </c>
       <c r="K13" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L13" s="9">
-        <f>J13*K13</f>
+        <f t="shared" si="2"/>
         <v>72.653100000000009</v>
       </c>
       <c r="M13" s="9">
-        <f>J13-L13</f>
+        <f t="shared" si="3"/>
         <v>1045.0869</v>
       </c>
     </row>
@@ -1800,7 +1800,7 @@
         <v>42484</v>
       </c>
       <c r="G14" s="8">
-        <f>F14-E14</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H14" s="2">
@@ -1810,18 +1810,18 @@
         <v>37.99</v>
       </c>
       <c r="J14" s="9">
-        <f>H14*I14</f>
+        <f t="shared" si="1"/>
         <v>721.81000000000006</v>
       </c>
       <c r="K14" s="10">
         <v>0.06</v>
       </c>
       <c r="L14" s="9">
-        <f>J14*K14</f>
+        <f t="shared" si="2"/>
         <v>43.308599999999998</v>
       </c>
       <c r="M14" s="9">
-        <f>J14-L14</f>
+        <f t="shared" si="3"/>
         <v>678.5014000000001</v>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
         <v>42490</v>
       </c>
       <c r="G15" s="8">
-        <f>F15-E15</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H15" s="2">
@@ -1855,18 +1855,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J15" s="9">
-        <f>H15*I15</f>
+        <f t="shared" si="1"/>
         <v>220.86999999999998</v>
       </c>
       <c r="K15" s="10">
         <v>0.05</v>
       </c>
       <c r="L15" s="9">
-        <f>J15*K15</f>
+        <f t="shared" si="2"/>
         <v>11.0435</v>
       </c>
       <c r="M15" s="9">
-        <f>J15-L15</f>
+        <f t="shared" si="3"/>
         <v>209.82649999999998</v>
       </c>
     </row>
@@ -1890,7 +1890,7 @@
         <v>42489</v>
       </c>
       <c r="G16" s="8">
-        <f>F16-E16</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H16" s="2">
@@ -1900,18 +1900,18 @@
         <v>37.99</v>
       </c>
       <c r="J16" s="9">
-        <f>H16*I16</f>
+        <f t="shared" si="1"/>
         <v>569.85</v>
       </c>
       <c r="K16" s="10">
         <v>0.05</v>
       </c>
       <c r="L16" s="9">
-        <f>J16*K16</f>
+        <f t="shared" si="2"/>
         <v>28.492500000000003</v>
       </c>
       <c r="M16" s="9">
-        <f>J16-L16</f>
+        <f t="shared" si="3"/>
         <v>541.35750000000007</v>
       </c>
     </row>
@@ -1935,7 +1935,7 @@
         <v>42514</v>
       </c>
       <c r="G17" s="8">
-        <f>F17-E17</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H17" s="2">
@@ -1945,18 +1945,18 @@
         <v>37.99</v>
       </c>
       <c r="J17" s="9">
-        <f>H17*I17</f>
+        <f t="shared" si="1"/>
         <v>911.76</v>
       </c>
       <c r="K17" s="10">
         <v>0.06</v>
       </c>
       <c r="L17" s="9">
-        <f>J17*K17</f>
+        <f t="shared" si="2"/>
         <v>54.705599999999997</v>
       </c>
       <c r="M17" s="9">
-        <f>J17-L17</f>
+        <f t="shared" si="3"/>
         <v>857.05439999999999</v>
       </c>
     </row>
@@ -1980,7 +1980,7 @@
         <v>42517</v>
       </c>
       <c r="G18" s="8">
-        <f>F18-E18</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H18" s="2">
@@ -1990,18 +1990,18 @@
         <v>32.99</v>
       </c>
       <c r="J18" s="9">
-        <f>H18*I18</f>
+        <f t="shared" si="1"/>
         <v>527.84</v>
       </c>
       <c r="K18" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L18" s="9">
-        <f>J18*K18</f>
+        <f t="shared" si="2"/>
         <v>39.588000000000001</v>
       </c>
       <c r="M18" s="9">
-        <f>J18-L18</f>
+        <f t="shared" si="3"/>
         <v>488.25200000000001</v>
       </c>
     </row>
@@ -2025,7 +2025,7 @@
         <v>42512</v>
       </c>
       <c r="G19" s="8">
-        <f>F19-E19</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H19" s="2">
@@ -2035,18 +2035,18 @@
         <v>23.99</v>
       </c>
       <c r="J19" s="9">
-        <f>H19*I19</f>
+        <f t="shared" si="1"/>
         <v>575.76</v>
       </c>
       <c r="K19" s="10">
         <v>0.05</v>
       </c>
       <c r="L19" s="9">
-        <f>J19*K19</f>
+        <f t="shared" si="2"/>
         <v>28.788</v>
       </c>
       <c r="M19" s="9">
-        <f>J19-L19</f>
+        <f t="shared" si="3"/>
         <v>546.97199999999998</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
         <v>42519</v>
       </c>
       <c r="G20" s="8">
-        <f>F20-E20</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H20" s="2">
@@ -2080,18 +2080,18 @@
         <v>21.99</v>
       </c>
       <c r="J20" s="9">
-        <f>H20*I20</f>
+        <f t="shared" si="1"/>
         <v>461.78999999999996</v>
       </c>
       <c r="K20" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L20" s="9">
-        <f>J20*K20</f>
+        <f t="shared" si="2"/>
         <v>34.634249999999994</v>
       </c>
       <c r="M20" s="9">
-        <f>J20-L20</f>
+        <f t="shared" si="3"/>
         <v>427.15574999999995</v>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
         <v>42520</v>
       </c>
       <c r="G21" s="8">
-        <f>F21-E21</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H21" s="2">
@@ -2125,18 +2125,18 @@
         <v>42.99</v>
       </c>
       <c r="J21" s="9">
-        <f>H21*I21</f>
+        <f t="shared" si="1"/>
         <v>1117.74</v>
       </c>
       <c r="K21" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L21" s="9">
-        <f>J21*K21</f>
+        <f t="shared" si="2"/>
         <v>78.241800000000012</v>
       </c>
       <c r="M21" s="9">
-        <f>J21-L21</f>
+        <f t="shared" si="3"/>
         <v>1039.4982</v>
       </c>
     </row>
@@ -2160,7 +2160,7 @@
         <v>42536</v>
       </c>
       <c r="G22" s="8">
-        <f>F22-E22</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H22" s="2">
@@ -2170,18 +2170,18 @@
         <v>42.99</v>
       </c>
       <c r="J22" s="9">
-        <f>H22*I22</f>
+        <f t="shared" si="1"/>
         <v>644.85</v>
       </c>
       <c r="K22" s="10">
         <v>0.05</v>
       </c>
       <c r="L22" s="9">
-        <f>J22*K22</f>
+        <f t="shared" si="2"/>
         <v>32.2425</v>
       </c>
       <c r="M22" s="9">
-        <f>J22-L22</f>
+        <f t="shared" si="3"/>
         <v>612.60750000000007</v>
       </c>
     </row>
@@ -2205,7 +2205,7 @@
         <v>42542</v>
       </c>
       <c r="G23" s="8">
-        <f>F23-E23</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H23" s="2">
@@ -2215,18 +2215,18 @@
         <v>42.99</v>
       </c>
       <c r="J23" s="9">
-        <f>H23*I23</f>
+        <f t="shared" si="1"/>
         <v>730.83</v>
       </c>
       <c r="K23" s="10">
         <v>0.06</v>
       </c>
       <c r="L23" s="9">
-        <f>J23*K23</f>
+        <f t="shared" si="2"/>
         <v>43.849800000000002</v>
       </c>
       <c r="M23" s="9">
-        <f>J23-L23</f>
+        <f t="shared" si="3"/>
         <v>686.98020000000008</v>
       </c>
     </row>
@@ -2250,7 +2250,7 @@
         <v>42373</v>
       </c>
       <c r="G24" s="8">
-        <f>F24-E24</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H24" s="2">
@@ -2260,18 +2260,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J24" s="9">
-        <f>H24*I24</f>
+        <f t="shared" si="1"/>
         <v>288.83</v>
       </c>
       <c r="K24" s="10">
         <v>0.06</v>
       </c>
       <c r="L24" s="9">
-        <f>J24*K24</f>
+        <f t="shared" si="2"/>
         <v>17.329799999999999</v>
       </c>
       <c r="M24" s="9">
-        <f>J24-L24</f>
+        <f t="shared" si="3"/>
         <v>271.50020000000001</v>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
         <v>42367</v>
       </c>
       <c r="G25" s="8">
-        <f>F25-E25</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H25" s="2">
@@ -2305,18 +2305,18 @@
         <v>49.99</v>
       </c>
       <c r="J25" s="9">
-        <f>H25*I25</f>
+        <f t="shared" si="1"/>
         <v>749.85</v>
       </c>
       <c r="K25" s="10">
         <v>0.06</v>
       </c>
       <c r="L25" s="9">
-        <f>J25*K25</f>
+        <f t="shared" si="2"/>
         <v>44.991</v>
       </c>
       <c r="M25" s="9">
-        <f>J25-L25</f>
+        <f t="shared" si="3"/>
         <v>704.85900000000004</v>
       </c>
     </row>
@@ -2340,7 +2340,7 @@
         <v>42368</v>
       </c>
       <c r="G26" s="8">
-        <f>F26-E26</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H26" s="2">
@@ -2350,18 +2350,18 @@
         <v>25.99</v>
       </c>
       <c r="J26" s="9">
-        <f>H26*I26</f>
+        <f t="shared" si="1"/>
         <v>623.76</v>
       </c>
       <c r="K26" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L26" s="9">
-        <f>J26*K26</f>
+        <f t="shared" si="2"/>
         <v>43.663200000000003</v>
       </c>
       <c r="M26" s="9">
-        <f>J26-L26</f>
+        <f t="shared" si="3"/>
         <v>580.09680000000003</v>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
         <v>42380</v>
       </c>
       <c r="G27" s="8">
-        <f>F27-E27</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="H27" s="2">
@@ -2395,18 +2395,18 @@
         <v>32.99</v>
       </c>
       <c r="J27" s="9">
-        <f>H27*I27</f>
+        <f t="shared" si="1"/>
         <v>593.82000000000005</v>
       </c>
       <c r="K27" s="10">
         <v>0.06</v>
       </c>
       <c r="L27" s="9">
-        <f>J27*K27</f>
+        <f t="shared" si="2"/>
         <v>35.629200000000004</v>
       </c>
       <c r="M27" s="9">
-        <f>J27-L27</f>
+        <f t="shared" si="3"/>
         <v>558.19080000000008</v>
       </c>
     </row>
@@ -2430,7 +2430,7 @@
         <v>42380</v>
       </c>
       <c r="G28" s="8">
-        <f>F28-E28</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H28" s="2">
@@ -2440,18 +2440,18 @@
         <v>37.99</v>
       </c>
       <c r="J28" s="9">
-        <f>H28*I28</f>
+        <f t="shared" si="1"/>
         <v>683.82</v>
       </c>
       <c r="K28" s="10">
         <v>0.05</v>
       </c>
       <c r="L28" s="9">
-        <f>J28*K28</f>
+        <f t="shared" si="2"/>
         <v>34.191000000000003</v>
       </c>
       <c r="M28" s="9">
-        <f>J28-L28</f>
+        <f t="shared" si="3"/>
         <v>649.62900000000002</v>
       </c>
     </row>
@@ -2475,7 +2475,7 @@
         <v>42380</v>
       </c>
       <c r="G29" s="8">
-        <f>F29-E29</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H29" s="2">
@@ -2485,18 +2485,18 @@
         <v>49.99</v>
       </c>
       <c r="J29" s="9">
-        <f>H29*I29</f>
+        <f t="shared" si="1"/>
         <v>1249.75</v>
       </c>
       <c r="K29" s="10">
         <v>0.06</v>
       </c>
       <c r="L29" s="9">
-        <f>J29*K29</f>
+        <f t="shared" si="2"/>
         <v>74.984999999999999</v>
       </c>
       <c r="M29" s="9">
-        <f>J29-L29</f>
+        <f t="shared" si="3"/>
         <v>1174.7650000000001</v>
       </c>
     </row>
@@ -2520,7 +2520,7 @@
         <v>42398</v>
       </c>
       <c r="G30" s="8">
-        <f>F30-E30</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H30" s="2">
@@ -2530,18 +2530,18 @@
         <v>23.99</v>
       </c>
       <c r="J30" s="9">
-        <f>H30*I30</f>
+        <f t="shared" si="1"/>
         <v>527.78</v>
       </c>
       <c r="K30" s="10">
         <v>0.06</v>
       </c>
       <c r="L30" s="9">
-        <f>J30*K30</f>
+        <f t="shared" si="2"/>
         <v>31.666799999999999</v>
       </c>
       <c r="M30" s="9">
-        <f>J30-L30</f>
+        <f t="shared" si="3"/>
         <v>496.11319999999995</v>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
         <v>42402</v>
       </c>
       <c r="G31" s="8">
-        <f>F31-E31</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="H31" s="2">
@@ -2575,18 +2575,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J31" s="9">
-        <f>H31*I31</f>
+        <f t="shared" si="1"/>
         <v>203.88</v>
       </c>
       <c r="K31" s="10">
         <v>0.06</v>
       </c>
       <c r="L31" s="9">
-        <f>J31*K31</f>
+        <f t="shared" si="2"/>
         <v>12.232799999999999</v>
       </c>
       <c r="M31" s="9">
-        <f>J31-L31</f>
+        <f t="shared" si="3"/>
         <v>191.6472</v>
       </c>
     </row>
@@ -2610,7 +2610,7 @@
         <v>42400</v>
       </c>
       <c r="G32" s="8">
-        <f>F32-E32</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H32" s="2">
@@ -2620,18 +2620,18 @@
         <v>9.99</v>
       </c>
       <c r="J32" s="9">
-        <f>H32*I32</f>
+        <f t="shared" si="1"/>
         <v>149.85</v>
       </c>
       <c r="K32" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L32" s="9">
-        <f>J32*K32</f>
+        <f t="shared" si="2"/>
         <v>11.23875</v>
       </c>
       <c r="M32" s="9">
-        <f>J32-L32</f>
+        <f t="shared" si="3"/>
         <v>138.61124999999998</v>
       </c>
     </row>
@@ -2655,7 +2655,7 @@
         <v>42411</v>
       </c>
       <c r="G33" s="8">
-        <f>F33-E33</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H33" s="2">
@@ -2665,18 +2665,18 @@
         <v>23.99</v>
       </c>
       <c r="J33" s="9">
-        <f>H33*I33</f>
+        <f t="shared" si="1"/>
         <v>431.82</v>
       </c>
       <c r="K33" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L33" s="9">
-        <f>J33*K33</f>
+        <f t="shared" si="2"/>
         <v>32.386499999999998</v>
       </c>
       <c r="M33" s="9">
-        <f>J33-L33</f>
+        <f t="shared" si="3"/>
         <v>399.43349999999998</v>
       </c>
     </row>
@@ -2700,7 +2700,7 @@
         <v>42417</v>
       </c>
       <c r="G34" s="8">
-        <f>F34-E34</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H34" s="2">
@@ -2710,18 +2710,18 @@
         <v>23.99</v>
       </c>
       <c r="J34" s="9">
-        <f>H34*I34</f>
+        <f t="shared" si="1"/>
         <v>599.75</v>
       </c>
       <c r="K34" s="10">
         <v>0.06</v>
       </c>
       <c r="L34" s="9">
-        <f>J34*K34</f>
+        <f t="shared" si="2"/>
         <v>35.984999999999999</v>
       </c>
       <c r="M34" s="9">
-        <f>J34-L34</f>
+        <f t="shared" si="3"/>
         <v>563.76499999999999</v>
       </c>
     </row>
@@ -2745,7 +2745,7 @@
         <v>42419</v>
       </c>
       <c r="G35" s="8">
-        <f>F35-E35</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H35" s="2">
@@ -2755,18 +2755,18 @@
         <v>23.99</v>
       </c>
       <c r="J35" s="9">
-        <f>H35*I35</f>
+        <f t="shared" si="1"/>
         <v>503.78999999999996</v>
       </c>
       <c r="K35" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L35" s="9">
-        <f>J35*K35</f>
+        <f t="shared" si="2"/>
         <v>35.265300000000003</v>
       </c>
       <c r="M35" s="9">
-        <f>J35-L35</f>
+        <f t="shared" si="3"/>
         <v>468.52469999999994</v>
       </c>
     </row>
@@ -2790,7 +2790,7 @@
         <v>42422</v>
       </c>
       <c r="G36" s="8">
-        <f>F36-E36</f>
+        <f t="shared" ref="G36:G67" si="4">F36-E36</f>
         <v>5</v>
       </c>
       <c r="H36" s="2">
@@ -2800,18 +2800,18 @@
         <v>42.99</v>
       </c>
       <c r="J36" s="9">
-        <f>H36*I36</f>
+        <f t="shared" ref="J36:J67" si="5">H36*I36</f>
         <v>515.88</v>
       </c>
       <c r="K36" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L36" s="9">
-        <f>J36*K36</f>
+        <f t="shared" ref="L36:L67" si="6">J36*K36</f>
         <v>36.111600000000003</v>
       </c>
       <c r="M36" s="9">
-        <f>J36-L36</f>
+        <f t="shared" ref="M36:M67" si="7">J36-L36</f>
         <v>479.76839999999999</v>
       </c>
     </row>
@@ -2835,7 +2835,7 @@
         <v>42436</v>
       </c>
       <c r="G37" s="8">
-        <f>F37-E37</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="H37" s="2">
@@ -2845,18 +2845,18 @@
         <v>32.99</v>
       </c>
       <c r="J37" s="9">
-        <f>H37*I37</f>
+        <f t="shared" si="5"/>
         <v>626.81000000000006</v>
       </c>
       <c r="K37" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L37" s="9">
-        <f>J37*K37</f>
+        <f t="shared" si="6"/>
         <v>47.010750000000002</v>
       </c>
       <c r="M37" s="9">
-        <f>J37-L37</f>
+        <f t="shared" si="7"/>
         <v>579.79925000000003</v>
       </c>
     </row>
@@ -2880,7 +2880,7 @@
         <v>42434</v>
       </c>
       <c r="G38" s="8">
-        <f>F38-E38</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H38" s="2">
@@ -2890,18 +2890,18 @@
         <v>9.99</v>
       </c>
       <c r="J38" s="9">
-        <f>H38*I38</f>
+        <f t="shared" si="5"/>
         <v>189.81</v>
       </c>
       <c r="K38" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L38" s="9">
-        <f>J38*K38</f>
+        <f t="shared" si="6"/>
         <v>13.286700000000002</v>
       </c>
       <c r="M38" s="9">
-        <f>J38-L38</f>
+        <f t="shared" si="7"/>
         <v>176.52330000000001</v>
       </c>
     </row>
@@ -2925,7 +2925,7 @@
         <v>42443</v>
       </c>
       <c r="G39" s="8">
-        <f>F39-E39</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H39" s="2">
@@ -2935,18 +2935,18 @@
         <v>49.99</v>
       </c>
       <c r="J39" s="9">
-        <f>H39*I39</f>
+        <f t="shared" si="5"/>
         <v>999.80000000000007</v>
       </c>
       <c r="K39" s="10">
         <v>0.05</v>
       </c>
       <c r="L39" s="9">
-        <f>J39*K39</f>
+        <f t="shared" si="6"/>
         <v>49.990000000000009</v>
       </c>
       <c r="M39" s="9">
-        <f>J39-L39</f>
+        <f t="shared" si="7"/>
         <v>949.81000000000006</v>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
         <v>42444</v>
       </c>
       <c r="G40" s="8">
-        <f>F40-E40</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H40" s="2">
@@ -2980,18 +2980,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J40" s="9">
-        <f>H40*I40</f>
+        <f t="shared" si="5"/>
         <v>339.79999999999995</v>
       </c>
       <c r="K40" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L40" s="9">
-        <f>J40*K40</f>
+        <f t="shared" si="6"/>
         <v>23.785999999999998</v>
       </c>
       <c r="M40" s="9">
-        <f>J40-L40</f>
+        <f t="shared" si="7"/>
         <v>316.01399999999995</v>
       </c>
     </row>
@@ -3015,7 +3015,7 @@
         <v>42455</v>
       </c>
       <c r="G41" s="8">
-        <f>F41-E41</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H41" s="2">
@@ -3025,18 +3025,18 @@
         <v>25.99</v>
       </c>
       <c r="J41" s="9">
-        <f>H41*I41</f>
+        <f t="shared" si="5"/>
         <v>363.85999999999996</v>
       </c>
       <c r="K41" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L41" s="9">
-        <f>J41*K41</f>
+        <f t="shared" si="6"/>
         <v>25.470199999999998</v>
       </c>
       <c r="M41" s="9">
-        <f>J41-L41</f>
+        <f t="shared" si="7"/>
         <v>338.38979999999998</v>
       </c>
     </row>
@@ -3060,7 +3060,7 @@
         <v>42468</v>
       </c>
       <c r="G42" s="8">
-        <f>F42-E42</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="H42" s="2">
@@ -3070,18 +3070,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J42" s="9">
-        <f>H42*I42</f>
+        <f t="shared" si="5"/>
         <v>424.74999999999994</v>
       </c>
       <c r="K42" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L42" s="9">
-        <f>J42*K42</f>
+        <f t="shared" si="6"/>
         <v>27.608749999999997</v>
       </c>
       <c r="M42" s="9">
-        <f>J42-L42</f>
+        <f t="shared" si="7"/>
         <v>397.14124999999996</v>
       </c>
     </row>
@@ -3105,7 +3105,7 @@
         <v>42474</v>
       </c>
       <c r="G43" s="8">
-        <f>F43-E43</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="H43" s="2">
@@ -3115,18 +3115,18 @@
         <v>25.99</v>
       </c>
       <c r="J43" s="9">
-        <f>H43*I43</f>
+        <f t="shared" si="5"/>
         <v>441.83</v>
       </c>
       <c r="K43" s="10">
         <v>0.05</v>
       </c>
       <c r="L43" s="9">
-        <f>J43*K43</f>
+        <f t="shared" si="6"/>
         <v>22.0915</v>
       </c>
       <c r="M43" s="9">
-        <f>J43-L43</f>
+        <f t="shared" si="7"/>
         <v>419.73849999999999</v>
       </c>
     </row>
@@ -3150,7 +3150,7 @@
         <v>42480</v>
       </c>
       <c r="G44" s="8">
-        <f>F44-E44</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H44" s="2">
@@ -3160,18 +3160,18 @@
         <v>23.99</v>
       </c>
       <c r="J44" s="9">
-        <f>H44*I44</f>
+        <f t="shared" si="5"/>
         <v>359.84999999999997</v>
       </c>
       <c r="K44" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L44" s="9">
-        <f>J44*K44</f>
+        <f t="shared" si="6"/>
         <v>25.189499999999999</v>
       </c>
       <c r="M44" s="9">
-        <f>J44-L44</f>
+        <f t="shared" si="7"/>
         <v>334.66049999999996</v>
       </c>
     </row>
@@ -3195,7 +3195,7 @@
         <v>42481</v>
       </c>
       <c r="G45" s="8">
-        <f>F45-E45</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H45" s="2">
@@ -3205,18 +3205,18 @@
         <v>32.99</v>
       </c>
       <c r="J45" s="9">
-        <f>H45*I45</f>
+        <f t="shared" si="5"/>
         <v>725.78000000000009</v>
       </c>
       <c r="K45" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L45" s="9">
-        <f>J45*K45</f>
+        <f t="shared" si="6"/>
         <v>50.804600000000008</v>
       </c>
       <c r="M45" s="9">
-        <f>J45-L45</f>
+        <f t="shared" si="7"/>
         <v>674.97540000000004</v>
       </c>
     </row>
@@ -3240,7 +3240,7 @@
         <v>42494</v>
       </c>
       <c r="G46" s="8">
-        <f>F46-E46</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H46" s="2">
@@ -3250,18 +3250,18 @@
         <v>9.99</v>
       </c>
       <c r="J46" s="9">
-        <f>H46*I46</f>
+        <f t="shared" si="5"/>
         <v>129.87</v>
       </c>
       <c r="K46" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L46" s="9">
-        <f>J46*K46</f>
+        <f t="shared" si="6"/>
         <v>8.4415500000000012</v>
       </c>
       <c r="M46" s="9">
-        <f>J46-L46</f>
+        <f t="shared" si="7"/>
         <v>121.42845</v>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
         <v>42503</v>
       </c>
       <c r="G47" s="8">
-        <f>F47-E47</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H47" s="2">
@@ -3295,18 +3295,18 @@
         <v>9.99</v>
       </c>
       <c r="J47" s="9">
-        <f>H47*I47</f>
+        <f t="shared" si="5"/>
         <v>229.77</v>
       </c>
       <c r="K47" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L47" s="9">
-        <f>J47*K47</f>
+        <f t="shared" si="6"/>
         <v>17.232749999999999</v>
       </c>
       <c r="M47" s="9">
-        <f>J47-L47</f>
+        <f t="shared" si="7"/>
         <v>212.53725</v>
       </c>
     </row>
@@ -3330,7 +3330,7 @@
         <v>42492</v>
       </c>
       <c r="G48" s="8">
-        <f>F48-E48</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H48" s="2">
@@ -3340,18 +3340,18 @@
         <v>9.99</v>
       </c>
       <c r="J48" s="9">
-        <f>H48*I48</f>
+        <f t="shared" si="5"/>
         <v>219.78</v>
       </c>
       <c r="K48" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L48" s="9">
-        <f>J48*K48</f>
+        <f t="shared" si="6"/>
         <v>16.483499999999999</v>
       </c>
       <c r="M48" s="9">
-        <f>J48-L48</f>
+        <f t="shared" si="7"/>
         <v>203.29650000000001</v>
       </c>
     </row>
@@ -3375,7 +3375,7 @@
         <v>42500</v>
       </c>
       <c r="G49" s="8">
-        <f>F49-E49</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H49" s="2">
@@ -3385,18 +3385,18 @@
         <v>25.99</v>
       </c>
       <c r="J49" s="9">
-        <f>H49*I49</f>
+        <f t="shared" si="5"/>
         <v>337.87</v>
       </c>
       <c r="K49" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L49" s="9">
-        <f>J49*K49</f>
+        <f t="shared" si="6"/>
         <v>23.650900000000004</v>
       </c>
       <c r="M49" s="9">
-        <f>J49-L49</f>
+        <f t="shared" si="7"/>
         <v>314.21910000000003</v>
       </c>
     </row>
@@ -3420,7 +3420,7 @@
         <v>42509</v>
       </c>
       <c r="G50" s="8">
-        <f>F50-E50</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="H50" s="2">
@@ -3430,18 +3430,18 @@
         <v>49.99</v>
       </c>
       <c r="J50" s="9">
-        <f>H50*I50</f>
+        <f t="shared" si="5"/>
         <v>1249.75</v>
       </c>
       <c r="K50" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L50" s="9">
-        <f>J50*K50</f>
+        <f t="shared" si="6"/>
         <v>81.233750000000001</v>
       </c>
       <c r="M50" s="9">
-        <f>J50-L50</f>
+        <f t="shared" si="7"/>
         <v>1168.5162499999999</v>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
         <v>42508</v>
       </c>
       <c r="G51" s="8">
-        <f>F51-E51</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="H51" s="2">
@@ -3475,18 +3475,18 @@
         <v>21.99</v>
       </c>
       <c r="J51" s="9">
-        <f>H51*I51</f>
+        <f t="shared" si="5"/>
         <v>593.7299999999999</v>
       </c>
       <c r="K51" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L51" s="9">
-        <f>J51*K51</f>
+        <f t="shared" si="6"/>
         <v>41.561099999999996</v>
       </c>
       <c r="M51" s="9">
-        <f>J51-L51</f>
+        <f t="shared" si="7"/>
         <v>552.16889999999989</v>
       </c>
     </row>
@@ -3510,7 +3510,7 @@
         <v>42519</v>
       </c>
       <c r="G52" s="8">
-        <f>F52-E52</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="H52" s="2">
@@ -3520,18 +3520,18 @@
         <v>37.99</v>
       </c>
       <c r="J52" s="9">
-        <f>H52*I52</f>
+        <f t="shared" si="5"/>
         <v>797.79000000000008</v>
       </c>
       <c r="K52" s="10">
         <v>0.05</v>
       </c>
       <c r="L52" s="9">
-        <f>J52*K52</f>
+        <f t="shared" si="6"/>
         <v>39.889500000000005</v>
       </c>
       <c r="M52" s="9">
-        <f>J52-L52</f>
+        <f t="shared" si="7"/>
         <v>757.90050000000008</v>
       </c>
     </row>
@@ -3555,7 +3555,7 @@
         <v>42521</v>
       </c>
       <c r="G53" s="8">
-        <f>F53-E53</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="H53" s="2">
@@ -3565,18 +3565,18 @@
         <v>9.99</v>
       </c>
       <c r="J53" s="9">
-        <f>H53*I53</f>
+        <f t="shared" si="5"/>
         <v>209.79</v>
       </c>
       <c r="K53" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L53" s="9">
-        <f>J53*K53</f>
+        <f t="shared" si="6"/>
         <v>15.734249999999999</v>
       </c>
       <c r="M53" s="9">
-        <f>J53-L53</f>
+        <f t="shared" si="7"/>
         <v>194.05574999999999</v>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
         <v>42529</v>
       </c>
       <c r="G54" s="8">
-        <f>F54-E54</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H54" s="2">
@@ -3610,18 +3610,18 @@
         <v>49.99</v>
       </c>
       <c r="J54" s="9">
-        <f>H54*I54</f>
+        <f t="shared" si="5"/>
         <v>1299.74</v>
       </c>
       <c r="K54" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L54" s="9">
-        <f>J54*K54</f>
+        <f t="shared" si="6"/>
         <v>84.483100000000007</v>
       </c>
       <c r="M54" s="9">
-        <f>J54-L54</f>
+        <f t="shared" si="7"/>
         <v>1215.2569000000001</v>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
         <v>42528</v>
       </c>
       <c r="G55" s="8">
-        <f>F55-E55</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="H55" s="2">
@@ -3655,18 +3655,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J55" s="9">
-        <f>H55*I55</f>
+        <f t="shared" si="5"/>
         <v>339.79999999999995</v>
       </c>
       <c r="K55" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L55" s="9">
-        <f>J55*K55</f>
+        <f t="shared" si="6"/>
         <v>25.484999999999996</v>
       </c>
       <c r="M55" s="9">
-        <f>J55-L55</f>
+        <f t="shared" si="7"/>
         <v>314.31499999999994</v>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
         <v>42530</v>
       </c>
       <c r="G56" s="8">
-        <f>F56-E56</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="H56" s="2">
@@ -3700,18 +3700,18 @@
         <v>42.99</v>
       </c>
       <c r="J56" s="9">
-        <f>H56*I56</f>
+        <f t="shared" si="5"/>
         <v>945.78000000000009</v>
       </c>
       <c r="K56" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L56" s="9">
-        <f>J56*K56</f>
+        <f t="shared" si="6"/>
         <v>61.47570000000001</v>
       </c>
       <c r="M56" s="9">
-        <f>J56-L56</f>
+        <f t="shared" si="7"/>
         <v>884.30430000000013</v>
       </c>
     </row>
@@ -3735,7 +3735,7 @@
         <v>42533</v>
       </c>
       <c r="G57" s="8">
-        <f>F57-E57</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="H57" s="2">
@@ -3745,18 +3745,18 @@
         <v>25.99</v>
       </c>
       <c r="J57" s="9">
-        <f>H57*I57</f>
+        <f t="shared" si="5"/>
         <v>337.87</v>
       </c>
       <c r="K57" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L57" s="9">
-        <f>J57*K57</f>
+        <f t="shared" si="6"/>
         <v>25.340250000000001</v>
       </c>
       <c r="M57" s="9">
-        <f>J57-L57</f>
+        <f t="shared" si="7"/>
         <v>312.52974999999998</v>
       </c>
     </row>
@@ -3780,7 +3780,7 @@
         <v>42543</v>
       </c>
       <c r="G58" s="8">
-        <f>F58-E58</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="H58" s="2">
@@ -3790,18 +3790,18 @@
         <v>37.99</v>
       </c>
       <c r="J58" s="9">
-        <f>H58*I58</f>
+        <f t="shared" si="5"/>
         <v>835.78000000000009</v>
       </c>
       <c r="K58" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L58" s="9">
-        <f>J58*K58</f>
+        <f t="shared" si="6"/>
         <v>62.683500000000002</v>
       </c>
       <c r="M58" s="9">
-        <f>J58-L58</f>
+        <f t="shared" si="7"/>
         <v>773.09650000000011</v>
       </c>
     </row>
@@ -3825,7 +3825,7 @@
         <v>42539</v>
       </c>
       <c r="G59" s="8">
-        <f>F59-E59</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="H59" s="2">
@@ -3835,18 +3835,18 @@
         <v>12.99</v>
       </c>
       <c r="J59" s="9">
-        <f>H59*I59</f>
+        <f t="shared" si="5"/>
         <v>311.76</v>
       </c>
       <c r="K59" s="10">
         <v>0.06</v>
       </c>
       <c r="L59" s="9">
-        <f>J59*K59</f>
+        <f t="shared" si="6"/>
         <v>18.7056</v>
       </c>
       <c r="M59" s="9">
-        <f>J59-L59</f>
+        <f t="shared" si="7"/>
         <v>293.05439999999999</v>
       </c>
     </row>
@@ -3870,7 +3870,7 @@
         <v>42550</v>
       </c>
       <c r="G60" s="8">
-        <f>F60-E60</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H60" s="2">
@@ -3880,18 +3880,18 @@
         <v>32.99</v>
       </c>
       <c r="J60" s="9">
-        <f>H60*I60</f>
+        <f t="shared" si="5"/>
         <v>461.86</v>
       </c>
       <c r="K60" s="10">
         <v>0.05</v>
       </c>
       <c r="L60" s="9">
-        <f>J60*K60</f>
+        <f t="shared" si="6"/>
         <v>23.093000000000004</v>
       </c>
       <c r="M60" s="9">
-        <f>J60-L60</f>
+        <f t="shared" si="7"/>
         <v>438.767</v>
       </c>
     </row>
@@ -3915,7 +3915,7 @@
         <v>42543</v>
       </c>
       <c r="G61" s="8">
-        <f>F61-E61</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H61" s="2">
@@ -3925,18 +3925,18 @@
         <v>9.99</v>
       </c>
       <c r="J61" s="9">
-        <f>H61*I61</f>
+        <f t="shared" si="5"/>
         <v>149.85</v>
       </c>
       <c r="K61" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L61" s="9">
-        <f>J61*K61</f>
+        <f t="shared" si="6"/>
         <v>11.23875</v>
       </c>
       <c r="M61" s="9">
-        <f>J61-L61</f>
+        <f t="shared" si="7"/>
         <v>138.61124999999998</v>
       </c>
     </row>
@@ -3960,7 +3960,7 @@
         <v>42366</v>
       </c>
       <c r="G62" s="8">
-        <f>F62-E62</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="H62" s="2">
@@ -3970,18 +3970,18 @@
         <v>21.99</v>
       </c>
       <c r="J62" s="9">
-        <f>H62*I62</f>
+        <f t="shared" si="5"/>
         <v>527.76</v>
       </c>
       <c r="K62" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L62" s="9">
-        <f>J62*K62</f>
+        <f t="shared" si="6"/>
         <v>36.943200000000004</v>
       </c>
       <c r="M62" s="9">
-        <f>J62-L62</f>
+        <f t="shared" si="7"/>
         <v>490.8168</v>
       </c>
     </row>
@@ -4005,7 +4005,7 @@
         <v>42370</v>
       </c>
       <c r="G63" s="8">
-        <f>F63-E63</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="H63" s="2">
@@ -4015,18 +4015,18 @@
         <v>21.99</v>
       </c>
       <c r="J63" s="9">
-        <f>H63*I63</f>
+        <f t="shared" si="5"/>
         <v>417.80999999999995</v>
       </c>
       <c r="K63" s="10">
         <v>0.06</v>
       </c>
       <c r="L63" s="9">
-        <f>J63*K63</f>
+        <f t="shared" si="6"/>
         <v>25.068599999999996</v>
       </c>
       <c r="M63" s="9">
-        <f>J63-L63</f>
+        <f t="shared" si="7"/>
         <v>392.74139999999994</v>
       </c>
     </row>
@@ -4050,7 +4050,7 @@
         <v>42365</v>
       </c>
       <c r="G64" s="8">
-        <f>F64-E64</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="H64" s="2">
@@ -4060,18 +4060,18 @@
         <v>49.99</v>
       </c>
       <c r="J64" s="9">
-        <f>H64*I64</f>
+        <f t="shared" si="5"/>
         <v>949.81000000000006</v>
       </c>
       <c r="K64" s="10">
         <v>0.05</v>
       </c>
       <c r="L64" s="9">
-        <f>J64*K64</f>
+        <f t="shared" si="6"/>
         <v>47.490500000000004</v>
       </c>
       <c r="M64" s="9">
-        <f>J64-L64</f>
+        <f t="shared" si="7"/>
         <v>902.31950000000006</v>
       </c>
     </row>
@@ -4095,7 +4095,7 @@
         <v>42364</v>
       </c>
       <c r="G65" s="8">
-        <f>F65-E65</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="H65" s="2">
@@ -4105,18 +4105,18 @@
         <v>25.99</v>
       </c>
       <c r="J65" s="9">
-        <f>H65*I65</f>
+        <f t="shared" si="5"/>
         <v>623.76</v>
       </c>
       <c r="K65" s="10">
         <v>0.06</v>
       </c>
       <c r="L65" s="9">
-        <f>J65*K65</f>
+        <f t="shared" si="6"/>
         <v>37.425599999999996</v>
       </c>
       <c r="M65" s="9">
-        <f>J65-L65</f>
+        <f t="shared" si="7"/>
         <v>586.33439999999996</v>
       </c>
     </row>
@@ -4140,7 +4140,7 @@
         <v>42363</v>
       </c>
       <c r="G66" s="8">
-        <f>F66-E66</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H66" s="2">
@@ -4150,18 +4150,18 @@
         <v>37.99</v>
       </c>
       <c r="J66" s="9">
-        <f>H66*I66</f>
+        <f t="shared" si="5"/>
         <v>493.87</v>
       </c>
       <c r="K66" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L66" s="9">
-        <f>J66*K66</f>
+        <f t="shared" si="6"/>
         <v>34.570900000000002</v>
       </c>
       <c r="M66" s="9">
-        <f>J66-L66</f>
+        <f t="shared" si="7"/>
         <v>459.29910000000001</v>
       </c>
     </row>
@@ -4185,7 +4185,7 @@
         <v>42368</v>
       </c>
       <c r="G67" s="8">
-        <f>F67-E67</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="H67" s="2">
@@ -4195,18 +4195,18 @@
         <v>49.99</v>
       </c>
       <c r="J67" s="9">
-        <f>H67*I67</f>
+        <f t="shared" si="5"/>
         <v>1099.78</v>
       </c>
       <c r="K67" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L67" s="9">
-        <f>J67*K67</f>
+        <f t="shared" si="6"/>
         <v>71.485699999999994</v>
       </c>
       <c r="M67" s="9">
-        <f>J67-L67</f>
+        <f t="shared" si="7"/>
         <v>1028.2943</v>
       </c>
     </row>
@@ -4230,7 +4230,7 @@
         <v>42377</v>
       </c>
       <c r="G68" s="8">
-        <f>F68-E68</f>
+        <f t="shared" ref="G68:G99" si="8">F68-E68</f>
         <v>12</v>
       </c>
       <c r="H68" s="2">
@@ -4240,18 +4240,18 @@
         <v>21.99</v>
       </c>
       <c r="J68" s="9">
-        <f>H68*I68</f>
+        <f t="shared" ref="J68:J99" si="9">H68*I68</f>
         <v>351.84</v>
       </c>
       <c r="K68" s="10">
         <v>0.05</v>
       </c>
       <c r="L68" s="9">
-        <f>J68*K68</f>
+        <f t="shared" ref="L68:L99" si="10">J68*K68</f>
         <v>17.591999999999999</v>
       </c>
       <c r="M68" s="9">
-        <f>J68-L68</f>
+        <f t="shared" ref="M68:M99" si="11">J68-L68</f>
         <v>334.24799999999999</v>
       </c>
     </row>
@@ -4275,7 +4275,7 @@
         <v>42372</v>
       </c>
       <c r="G69" s="8">
-        <f>F69-E69</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="H69" s="2">
@@ -4285,18 +4285,18 @@
         <v>49.99</v>
       </c>
       <c r="J69" s="9">
-        <f>H69*I69</f>
+        <f t="shared" si="9"/>
         <v>1249.75</v>
       </c>
       <c r="K69" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L69" s="9">
-        <f>J69*K69</f>
+        <f t="shared" si="10"/>
         <v>93.731250000000003</v>
       </c>
       <c r="M69" s="9">
-        <f>J69-L69</f>
+        <f t="shared" si="11"/>
         <v>1156.01875</v>
       </c>
     </row>
@@ -4320,7 +4320,7 @@
         <v>42376</v>
       </c>
       <c r="G70" s="8">
-        <f>F70-E70</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="H70" s="2">
@@ -4330,18 +4330,18 @@
         <v>21.99</v>
       </c>
       <c r="J70" s="9">
-        <f>H70*I70</f>
+        <f t="shared" si="9"/>
         <v>439.79999999999995</v>
       </c>
       <c r="K70" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L70" s="9">
-        <f>J70*K70</f>
+        <f t="shared" si="10"/>
         <v>28.587</v>
       </c>
       <c r="M70" s="9">
-        <f>J70-L70</f>
+        <f t="shared" si="11"/>
         <v>411.21299999999997</v>
       </c>
     </row>
@@ -4365,7 +4365,7 @@
         <v>42380</v>
       </c>
       <c r="G71" s="8">
-        <f>F71-E71</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="H71" s="2">
@@ -4375,18 +4375,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J71" s="9">
-        <f>H71*I71</f>
+        <f t="shared" si="9"/>
         <v>203.88</v>
       </c>
       <c r="K71" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L71" s="9">
-        <f>J71*K71</f>
+        <f t="shared" si="10"/>
         <v>15.290999999999999</v>
       </c>
       <c r="M71" s="9">
-        <f>J71-L71</f>
+        <f t="shared" si="11"/>
         <v>188.589</v>
       </c>
     </row>
@@ -4410,7 +4410,7 @@
         <v>42374</v>
       </c>
       <c r="G72" s="8">
-        <f>F72-E72</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H72" s="2">
@@ -4420,18 +4420,18 @@
         <v>21.99</v>
       </c>
       <c r="J72" s="9">
-        <f>H72*I72</f>
+        <f t="shared" si="9"/>
         <v>329.84999999999997</v>
       </c>
       <c r="K72" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L72" s="9">
-        <f>J72*K72</f>
+        <f t="shared" si="10"/>
         <v>23.089500000000001</v>
       </c>
       <c r="M72" s="9">
-        <f>J72-L72</f>
+        <f t="shared" si="11"/>
         <v>306.76049999999998</v>
       </c>
     </row>
@@ -4455,7 +4455,7 @@
         <v>42384</v>
       </c>
       <c r="G73" s="8">
-        <f>F73-E73</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="H73" s="2">
@@ -4465,18 +4465,18 @@
         <v>21.99</v>
       </c>
       <c r="J73" s="9">
-        <f>H73*I73</f>
+        <f t="shared" si="9"/>
         <v>483.78</v>
       </c>
       <c r="K73" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L73" s="9">
-        <f>J73*K73</f>
+        <f t="shared" si="10"/>
         <v>31.445699999999999</v>
       </c>
       <c r="M73" s="9">
-        <f>J73-L73</f>
+        <f t="shared" si="11"/>
         <v>452.33429999999998</v>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
         <v>42388</v>
       </c>
       <c r="G74" s="8">
-        <f>F74-E74</f>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="H74" s="2">
@@ -4510,18 +4510,18 @@
         <v>9.99</v>
       </c>
       <c r="J74" s="9">
-        <f>H74*I74</f>
+        <f t="shared" si="9"/>
         <v>209.79</v>
       </c>
       <c r="K74" s="10">
         <v>0.05</v>
       </c>
       <c r="L74" s="9">
-        <f>J74*K74</f>
+        <f t="shared" si="10"/>
         <v>10.4895</v>
       </c>
       <c r="M74" s="9">
-        <f>J74-L74</f>
+        <f t="shared" si="11"/>
         <v>199.3005</v>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
         <v>42394</v>
       </c>
       <c r="G75" s="8">
-        <f>F75-E75</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="H75" s="2">
@@ -4555,18 +4555,18 @@
         <v>42.99</v>
       </c>
       <c r="J75" s="9">
-        <f>H75*I75</f>
+        <f t="shared" si="9"/>
         <v>1074.75</v>
       </c>
       <c r="K75" s="10">
         <v>0.05</v>
       </c>
       <c r="L75" s="9">
-        <f>J75*K75</f>
+        <f t="shared" si="10"/>
         <v>53.737500000000004</v>
       </c>
       <c r="M75" s="9">
-        <f>J75-L75</f>
+        <f t="shared" si="11"/>
         <v>1021.0125</v>
       </c>
     </row>
@@ -4590,7 +4590,7 @@
         <v>42398</v>
       </c>
       <c r="G76" s="8">
-        <f>F76-E76</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="H76" s="2">
@@ -4600,18 +4600,18 @@
         <v>49.99</v>
       </c>
       <c r="J76" s="9">
-        <f>H76*I76</f>
+        <f t="shared" si="9"/>
         <v>1099.78</v>
       </c>
       <c r="K76" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L76" s="9">
-        <f>J76*K76</f>
+        <f t="shared" si="10"/>
         <v>76.9846</v>
       </c>
       <c r="M76" s="9">
-        <f>J76-L76</f>
+        <f t="shared" si="11"/>
         <v>1022.7954</v>
       </c>
     </row>
@@ -4635,7 +4635,7 @@
         <v>42393</v>
       </c>
       <c r="G77" s="8">
-        <f>F77-E77</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="H77" s="2">
@@ -4645,18 +4645,18 @@
         <v>32.99</v>
       </c>
       <c r="J77" s="9">
-        <f>H77*I77</f>
+        <f t="shared" si="9"/>
         <v>461.86</v>
       </c>
       <c r="K77" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L77" s="9">
-        <f>J77*K77</f>
+        <f t="shared" si="10"/>
         <v>32.330200000000005</v>
       </c>
       <c r="M77" s="9">
-        <f>J77-L77</f>
+        <f t="shared" si="11"/>
         <v>429.52980000000002</v>
       </c>
     </row>
@@ -4680,7 +4680,7 @@
         <v>42399</v>
       </c>
       <c r="G78" s="8">
-        <f>F78-E78</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="H78" s="2">
@@ -4690,18 +4690,18 @@
         <v>25.99</v>
       </c>
       <c r="J78" s="9">
-        <f>H78*I78</f>
+        <f t="shared" si="9"/>
         <v>337.87</v>
       </c>
       <c r="K78" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L78" s="9">
-        <f>J78*K78</f>
+        <f t="shared" si="10"/>
         <v>23.650900000000004</v>
       </c>
       <c r="M78" s="9">
-        <f>J78-L78</f>
+        <f t="shared" si="11"/>
         <v>314.21910000000003</v>
       </c>
     </row>
@@ -4725,7 +4725,7 @@
         <v>42399</v>
       </c>
       <c r="G79" s="8">
-        <f>F79-E79</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H79" s="2">
@@ -4735,18 +4735,18 @@
         <v>23.99</v>
       </c>
       <c r="J79" s="9">
-        <f>H79*I79</f>
+        <f t="shared" si="9"/>
         <v>551.77</v>
       </c>
       <c r="K79" s="10">
         <v>0.05</v>
       </c>
       <c r="L79" s="9">
-        <f>J79*K79</f>
+        <f t="shared" si="10"/>
         <v>27.5885</v>
       </c>
       <c r="M79" s="9">
-        <f>J79-L79</f>
+        <f t="shared" si="11"/>
         <v>524.18150000000003</v>
       </c>
     </row>
@@ -4770,7 +4770,7 @@
         <v>42409</v>
       </c>
       <c r="G80" s="8">
-        <f>F80-E80</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="H80" s="2">
@@ -4780,18 +4780,18 @@
         <v>21.99</v>
       </c>
       <c r="J80" s="9">
-        <f>H80*I80</f>
+        <f t="shared" si="9"/>
         <v>461.78999999999996</v>
       </c>
       <c r="K80" s="10">
         <v>0.05</v>
       </c>
       <c r="L80" s="9">
-        <f>J80*K80</f>
+        <f t="shared" si="10"/>
         <v>23.089500000000001</v>
       </c>
       <c r="M80" s="9">
-        <f>J80-L80</f>
+        <f t="shared" si="11"/>
         <v>438.70049999999998</v>
       </c>
     </row>
@@ -4815,7 +4815,7 @@
         <v>42405</v>
       </c>
       <c r="G81" s="8">
-        <f>F81-E81</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="H81" s="2">
@@ -4825,18 +4825,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J81" s="9">
-        <f>H81*I81</f>
+        <f t="shared" si="9"/>
         <v>356.78999999999996</v>
       </c>
       <c r="K81" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L81" s="9">
-        <f>J81*K81</f>
+        <f t="shared" si="10"/>
         <v>26.759249999999998</v>
       </c>
       <c r="M81" s="9">
-        <f>J81-L81</f>
+        <f t="shared" si="11"/>
         <v>330.03074999999995</v>
       </c>
     </row>
@@ -4860,7 +4860,7 @@
         <v>42409</v>
       </c>
       <c r="G82" s="8">
-        <f>F82-E82</f>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="H82" s="2">
@@ -4870,18 +4870,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J82" s="9">
-        <f>H82*I82</f>
+        <f t="shared" si="9"/>
         <v>322.80999999999995</v>
       </c>
       <c r="K82" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L82" s="9">
-        <f>J82*K82</f>
+        <f t="shared" si="10"/>
         <v>20.982649999999996</v>
       </c>
       <c r="M82" s="9">
-        <f>J82-L82</f>
+        <f t="shared" si="11"/>
         <v>301.82734999999997</v>
       </c>
     </row>
@@ -4905,7 +4905,7 @@
         <v>42411</v>
       </c>
       <c r="G83" s="8">
-        <f>F83-E83</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H83" s="2">
@@ -4915,18 +4915,18 @@
         <v>9.99</v>
       </c>
       <c r="J83" s="9">
-        <f>H83*I83</f>
+        <f t="shared" si="9"/>
         <v>269.73</v>
       </c>
       <c r="K83" s="10">
         <v>0.05</v>
       </c>
       <c r="L83" s="9">
-        <f>J83*K83</f>
+        <f t="shared" si="10"/>
         <v>13.486500000000001</v>
       </c>
       <c r="M83" s="9">
-        <f>J83-L83</f>
+        <f t="shared" si="11"/>
         <v>256.24350000000004</v>
       </c>
     </row>
@@ -4950,7 +4950,7 @@
         <v>42416</v>
       </c>
       <c r="G84" s="8">
-        <f>F84-E84</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="H84" s="2">
@@ -4960,18 +4960,18 @@
         <v>23.99</v>
       </c>
       <c r="J84" s="9">
-        <f>H84*I84</f>
+        <f t="shared" si="9"/>
         <v>455.80999999999995</v>
       </c>
       <c r="K84" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L84" s="9">
-        <f>J84*K84</f>
+        <f t="shared" si="10"/>
         <v>29.627649999999999</v>
       </c>
       <c r="M84" s="9">
-        <f>J84-L84</f>
+        <f t="shared" si="11"/>
         <v>426.18234999999993</v>
       </c>
     </row>
@@ -4995,7 +4995,7 @@
         <v>42417</v>
       </c>
       <c r="G85" s="8">
-        <f>F85-E85</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H85" s="2">
@@ -5005,18 +5005,18 @@
         <v>21.99</v>
       </c>
       <c r="J85" s="9">
-        <f>H85*I85</f>
+        <f t="shared" si="9"/>
         <v>263.88</v>
       </c>
       <c r="K85" s="10">
         <v>0.05</v>
       </c>
       <c r="L85" s="9">
-        <f>J85*K85</f>
+        <f t="shared" si="10"/>
         <v>13.194000000000001</v>
       </c>
       <c r="M85" s="9">
-        <f>J85-L85</f>
+        <f t="shared" si="11"/>
         <v>250.68600000000001</v>
       </c>
     </row>
@@ -5040,7 +5040,7 @@
         <v>42429</v>
       </c>
       <c r="G86" s="8">
-        <f>F86-E86</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="H86" s="2">
@@ -5050,18 +5050,18 @@
         <v>32.99</v>
       </c>
       <c r="J86" s="9">
-        <f>H86*I86</f>
+        <f t="shared" si="9"/>
         <v>890.73</v>
       </c>
       <c r="K86" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L86" s="9">
-        <f>J86*K86</f>
+        <f t="shared" si="10"/>
         <v>57.897450000000006</v>
       </c>
       <c r="M86" s="9">
-        <f>J86-L86</f>
+        <f t="shared" si="11"/>
         <v>832.83254999999997</v>
       </c>
     </row>
@@ -5085,7 +5085,7 @@
         <v>42431</v>
       </c>
       <c r="G87" s="8">
-        <f>F87-E87</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="H87" s="2">
@@ -5095,18 +5095,18 @@
         <v>25.99</v>
       </c>
       <c r="J87" s="9">
-        <f>H87*I87</f>
+        <f t="shared" si="9"/>
         <v>701.7299999999999</v>
       </c>
       <c r="K87" s="10">
         <v>0.05</v>
       </c>
       <c r="L87" s="9">
-        <f>J87*K87</f>
+        <f t="shared" si="10"/>
         <v>35.086499999999994</v>
       </c>
       <c r="M87" s="9">
-        <f>J87-L87</f>
+        <f t="shared" si="11"/>
         <v>666.6434999999999</v>
       </c>
     </row>
@@ -5130,7 +5130,7 @@
         <v>42423</v>
       </c>
       <c r="G88" s="8">
-        <f>F88-E88</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H88" s="2">
@@ -5140,18 +5140,18 @@
         <v>21.99</v>
       </c>
       <c r="J88" s="9">
-        <f>H88*I88</f>
+        <f t="shared" si="9"/>
         <v>351.84</v>
       </c>
       <c r="K88" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L88" s="9">
-        <f>J88*K88</f>
+        <f t="shared" si="10"/>
         <v>26.387999999999998</v>
       </c>
       <c r="M88" s="9">
-        <f>J88-L88</f>
+        <f t="shared" si="11"/>
         <v>325.452</v>
       </c>
     </row>
@@ -5175,7 +5175,7 @@
         <v>42437</v>
       </c>
       <c r="G89" s="8">
-        <f>F89-E89</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="H89" s="2">
@@ -5185,18 +5185,18 @@
         <v>21.99</v>
       </c>
       <c r="J89" s="9">
-        <f>H89*I89</f>
+        <f t="shared" si="9"/>
         <v>307.85999999999996</v>
       </c>
       <c r="K89" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L89" s="9">
-        <f>J89*K89</f>
+        <f t="shared" si="10"/>
         <v>21.5502</v>
       </c>
       <c r="M89" s="9">
-        <f>J89-L89</f>
+        <f t="shared" si="11"/>
         <v>286.30979999999994</v>
       </c>
     </row>
@@ -5220,7 +5220,7 @@
         <v>42434</v>
       </c>
       <c r="G90" s="8">
-        <f>F90-E90</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="H90" s="2">
@@ -5230,18 +5230,18 @@
         <v>49.99</v>
       </c>
       <c r="J90" s="9">
-        <f>H90*I90</f>
+        <f t="shared" si="9"/>
         <v>699.86</v>
       </c>
       <c r="K90" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L90" s="9">
-        <f>J90*K90</f>
+        <f t="shared" si="10"/>
         <v>45.490900000000003</v>
       </c>
       <c r="M90" s="9">
-        <f>J90-L90</f>
+        <f t="shared" si="11"/>
         <v>654.3691</v>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
         <v>42430</v>
       </c>
       <c r="G91" s="8">
-        <f>F91-E91</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="H91" s="2">
@@ -5275,18 +5275,18 @@
         <v>23.99</v>
       </c>
       <c r="J91" s="9">
-        <f>H91*I91</f>
+        <f t="shared" si="9"/>
         <v>431.82</v>
       </c>
       <c r="K91" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L91" s="9">
-        <f>J91*K91</f>
+        <f t="shared" si="10"/>
         <v>32.386499999999998</v>
       </c>
       <c r="M91" s="9">
-        <f>J91-L91</f>
+        <f t="shared" si="11"/>
         <v>399.43349999999998</v>
       </c>
     </row>
@@ -5310,7 +5310,7 @@
         <v>42430</v>
       </c>
       <c r="G92" s="8">
-        <f>F92-E92</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H92" s="2">
@@ -5320,18 +5320,18 @@
         <v>49.99</v>
       </c>
       <c r="J92" s="9">
-        <f>H92*I92</f>
+        <f t="shared" si="9"/>
         <v>849.83</v>
       </c>
       <c r="K92" s="10">
         <v>0.05</v>
       </c>
       <c r="L92" s="9">
-        <f>J92*K92</f>
+        <f t="shared" si="10"/>
         <v>42.491500000000002</v>
       </c>
       <c r="M92" s="9">
-        <f>J92-L92</f>
+        <f t="shared" si="11"/>
         <v>807.33850000000007</v>
       </c>
     </row>
@@ -5355,7 +5355,7 @@
         <v>42443</v>
       </c>
       <c r="G93" s="8">
-        <f>F93-E93</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="H93" s="2">
@@ -5365,18 +5365,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J93" s="9">
-        <f>H93*I93</f>
+        <f t="shared" si="9"/>
         <v>407.76</v>
       </c>
       <c r="K93" s="10">
         <v>0.06</v>
       </c>
       <c r="L93" s="9">
-        <f>J93*K93</f>
+        <f t="shared" si="10"/>
         <v>24.465599999999998</v>
       </c>
       <c r="M93" s="9">
-        <f>J93-L93</f>
+        <f t="shared" si="11"/>
         <v>383.2944</v>
       </c>
     </row>
@@ -5400,7 +5400,7 @@
         <v>42432</v>
       </c>
       <c r="G94" s="8">
-        <f>F94-E94</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="H94" s="2">
@@ -5410,18 +5410,18 @@
         <v>12.99</v>
       </c>
       <c r="J94" s="9">
-        <f>H94*I94</f>
+        <f t="shared" si="9"/>
         <v>233.82</v>
       </c>
       <c r="K94" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L94" s="9">
-        <f>J94*K94</f>
+        <f t="shared" si="10"/>
         <v>17.5365</v>
       </c>
       <c r="M94" s="9">
-        <f>J94-L94</f>
+        <f t="shared" si="11"/>
         <v>216.2835</v>
       </c>
     </row>
@@ -5445,7 +5445,7 @@
         <v>42439</v>
       </c>
       <c r="G95" s="8">
-        <f>F95-E95</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="H95" s="2">
@@ -5455,18 +5455,18 @@
         <v>9.99</v>
       </c>
       <c r="J95" s="9">
-        <f>H95*I95</f>
+        <f t="shared" si="9"/>
         <v>179.82</v>
       </c>
       <c r="K95" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L95" s="9">
-        <f>J95*K95</f>
+        <f t="shared" si="10"/>
         <v>12.587400000000001</v>
       </c>
       <c r="M95" s="9">
-        <f>J95-L95</f>
+        <f t="shared" si="11"/>
         <v>167.23259999999999</v>
       </c>
     </row>
@@ -5490,7 +5490,7 @@
         <v>42442</v>
       </c>
       <c r="G96" s="8">
-        <f>F96-E96</f>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="H96" s="2">
@@ -5500,18 +5500,18 @@
         <v>12.99</v>
       </c>
       <c r="J96" s="9">
-        <f>H96*I96</f>
+        <f t="shared" si="9"/>
         <v>324.75</v>
       </c>
       <c r="K96" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L96" s="9">
-        <f>J96*K96</f>
+        <f t="shared" si="10"/>
         <v>22.732500000000002</v>
       </c>
       <c r="M96" s="9">
-        <f>J96-L96</f>
+        <f t="shared" si="11"/>
         <v>302.01749999999998</v>
       </c>
     </row>
@@ -5535,7 +5535,7 @@
         <v>42460</v>
       </c>
       <c r="G97" s="8">
-        <f>F97-E97</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="H97" s="2">
@@ -5545,18 +5545,18 @@
         <v>25.99</v>
       </c>
       <c r="J97" s="9">
-        <f>H97*I97</f>
+        <f t="shared" si="9"/>
         <v>389.84999999999997</v>
       </c>
       <c r="K97" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L97" s="9">
-        <f>J97*K97</f>
+        <f t="shared" si="10"/>
         <v>27.2895</v>
       </c>
       <c r="M97" s="9">
-        <f>J97-L97</f>
+        <f t="shared" si="11"/>
         <v>362.56049999999999</v>
       </c>
     </row>
@@ -5580,7 +5580,7 @@
         <v>42462</v>
       </c>
       <c r="G98" s="8">
-        <f>F98-E98</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="H98" s="2">
@@ -5590,18 +5590,18 @@
         <v>25.99</v>
       </c>
       <c r="J98" s="9">
-        <f>H98*I98</f>
+        <f t="shared" si="9"/>
         <v>597.77</v>
       </c>
       <c r="K98" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L98" s="9">
-        <f>J98*K98</f>
+        <f t="shared" si="10"/>
         <v>44.832749999999997</v>
       </c>
       <c r="M98" s="9">
-        <f>J98-L98</f>
+        <f t="shared" si="11"/>
         <v>552.93724999999995</v>
       </c>
     </row>
@@ -5625,7 +5625,7 @@
         <v>42456</v>
       </c>
       <c r="G99" s="8">
-        <f>F99-E99</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="H99" s="2">
@@ -5635,18 +5635,18 @@
         <v>25.99</v>
       </c>
       <c r="J99" s="9">
-        <f>H99*I99</f>
+        <f t="shared" si="9"/>
         <v>441.83</v>
       </c>
       <c r="K99" s="10">
         <v>0.06</v>
       </c>
       <c r="L99" s="9">
-        <f>J99*K99</f>
+        <f t="shared" si="10"/>
         <v>26.509799999999998</v>
       </c>
       <c r="M99" s="9">
-        <f>J99-L99</f>
+        <f t="shared" si="11"/>
         <v>415.3202</v>
       </c>
     </row>
@@ -5670,7 +5670,7 @@
         <v>42461</v>
       </c>
       <c r="G100" s="8">
-        <f>F100-E100</f>
+        <f t="shared" ref="G100:G131" si="12">F100-E100</f>
         <v>6</v>
       </c>
       <c r="H100" s="2">
@@ -5680,18 +5680,18 @@
         <v>9.99</v>
       </c>
       <c r="J100" s="9">
-        <f>H100*I100</f>
+        <f t="shared" ref="J100:J131" si="13">H100*I100</f>
         <v>219.78</v>
       </c>
       <c r="K100" s="10">
         <v>0.05</v>
       </c>
       <c r="L100" s="9">
-        <f>J100*K100</f>
+        <f t="shared" ref="L100:L131" si="14">J100*K100</f>
         <v>10.989000000000001</v>
       </c>
       <c r="M100" s="9">
-        <f>J100-L100</f>
+        <f t="shared" ref="M100:M131" si="15">J100-L100</f>
         <v>208.791</v>
       </c>
     </row>
@@ -5715,7 +5715,7 @@
         <v>42472</v>
       </c>
       <c r="G101" s="8">
-        <f>F101-E101</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="H101" s="2">
@@ -5725,18 +5725,18 @@
         <v>12.99</v>
       </c>
       <c r="J101" s="9">
-        <f>H101*I101</f>
+        <f t="shared" si="13"/>
         <v>337.74</v>
       </c>
       <c r="K101" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L101" s="9">
-        <f>J101*K101</f>
+        <f t="shared" si="14"/>
         <v>25.330500000000001</v>
       </c>
       <c r="M101" s="9">
-        <f>J101-L101</f>
+        <f t="shared" si="15"/>
         <v>312.40949999999998</v>
       </c>
     </row>
@@ -5760,7 +5760,7 @@
         <v>42478</v>
       </c>
       <c r="G102" s="8">
-        <f>F102-E102</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H102" s="2">
@@ -5770,18 +5770,18 @@
         <v>25.99</v>
       </c>
       <c r="J102" s="9">
-        <f>H102*I102</f>
+        <f t="shared" si="13"/>
         <v>493.80999999999995</v>
       </c>
       <c r="K102" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L102" s="9">
-        <f>J102*K102</f>
+        <f t="shared" si="14"/>
         <v>34.566699999999997</v>
       </c>
       <c r="M102" s="9">
-        <f>J102-L102</f>
+        <f t="shared" si="15"/>
         <v>459.24329999999998</v>
       </c>
     </row>
@@ -5805,7 +5805,7 @@
         <v>42485</v>
       </c>
       <c r="G103" s="8">
-        <f>F103-E103</f>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="H103" s="2">
@@ -5815,18 +5815,18 @@
         <v>42.99</v>
       </c>
       <c r="J103" s="9">
-        <f>H103*I103</f>
+        <f t="shared" si="13"/>
         <v>859.80000000000007</v>
       </c>
       <c r="K103" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L103" s="9">
-        <f>J103*K103</f>
+        <f t="shared" si="14"/>
         <v>64.484999999999999</v>
       </c>
       <c r="M103" s="9">
-        <f>J103-L103</f>
+        <f t="shared" si="15"/>
         <v>795.31500000000005</v>
       </c>
     </row>
@@ -5850,7 +5850,7 @@
         <v>42477</v>
       </c>
       <c r="G104" s="8">
-        <f>F104-E104</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="H104" s="2">
@@ -5860,18 +5860,18 @@
         <v>12.99</v>
       </c>
       <c r="J104" s="9">
-        <f>H104*I104</f>
+        <f t="shared" si="13"/>
         <v>233.82</v>
       </c>
       <c r="K104" s="10">
         <v>0.06</v>
       </c>
       <c r="L104" s="9">
-        <f>J104*K104</f>
+        <f t="shared" si="14"/>
         <v>14.029199999999999</v>
       </c>
       <c r="M104" s="9">
-        <f>J104-L104</f>
+        <f t="shared" si="15"/>
         <v>219.79079999999999</v>
       </c>
     </row>
@@ -5895,7 +5895,7 @@
         <v>42484</v>
       </c>
       <c r="G105" s="8">
-        <f>F105-E105</f>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="H105" s="2">
@@ -5905,18 +5905,18 @@
         <v>37.99</v>
       </c>
       <c r="J105" s="9">
-        <f>H105*I105</f>
+        <f t="shared" si="13"/>
         <v>493.87</v>
       </c>
       <c r="K105" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L105" s="9">
-        <f>J105*K105</f>
+        <f t="shared" si="14"/>
         <v>34.570900000000002</v>
       </c>
       <c r="M105" s="9">
-        <f>J105-L105</f>
+        <f t="shared" si="15"/>
         <v>459.29910000000001</v>
       </c>
     </row>
@@ -5940,7 +5940,7 @@
         <v>42479</v>
       </c>
       <c r="G106" s="8">
-        <f>F106-E106</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="H106" s="2">
@@ -5950,18 +5950,18 @@
         <v>49.99</v>
       </c>
       <c r="J106" s="9">
-        <f>H106*I106</f>
+        <f t="shared" si="13"/>
         <v>1249.75</v>
       </c>
       <c r="K106" s="10">
         <v>0.06</v>
       </c>
       <c r="L106" s="9">
-        <f>J106*K106</f>
+        <f t="shared" si="14"/>
         <v>74.984999999999999</v>
       </c>
       <c r="M106" s="9">
-        <f>J106-L106</f>
+        <f t="shared" si="15"/>
         <v>1174.7650000000001</v>
       </c>
     </row>
@@ -5985,7 +5985,7 @@
         <v>42493</v>
       </c>
       <c r="G107" s="8">
-        <f>F107-E107</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="H107" s="2">
@@ -5995,18 +5995,18 @@
         <v>9.99</v>
       </c>
       <c r="J107" s="9">
-        <f>H107*I107</f>
+        <f t="shared" si="13"/>
         <v>259.74</v>
       </c>
       <c r="K107" s="10">
         <v>0.06</v>
       </c>
       <c r="L107" s="9">
-        <f>J107*K107</f>
+        <f t="shared" si="14"/>
         <v>15.5844</v>
       </c>
       <c r="M107" s="9">
-        <f>J107-L107</f>
+        <f t="shared" si="15"/>
         <v>244.15560000000002</v>
       </c>
     </row>
@@ -6030,7 +6030,7 @@
         <v>42498</v>
       </c>
       <c r="G108" s="8">
-        <f>F108-E108</f>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="H108" s="2">
@@ -6040,18 +6040,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J108" s="9">
-        <f>H108*I108</f>
+        <f t="shared" si="13"/>
         <v>407.76</v>
       </c>
       <c r="K108" s="10">
         <v>0.06</v>
       </c>
       <c r="L108" s="9">
-        <f>J108*K108</f>
+        <f t="shared" si="14"/>
         <v>24.465599999999998</v>
       </c>
       <c r="M108" s="9">
-        <f>J108-L108</f>
+        <f t="shared" si="15"/>
         <v>383.2944</v>
       </c>
     </row>
@@ -6075,7 +6075,7 @@
         <v>42489</v>
       </c>
       <c r="G109" s="8">
-        <f>F109-E109</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H109" s="2">
@@ -6085,18 +6085,18 @@
         <v>12.99</v>
       </c>
       <c r="J109" s="9">
-        <f>H109*I109</f>
+        <f t="shared" si="13"/>
         <v>324.75</v>
       </c>
       <c r="K109" s="10">
         <v>0.05</v>
       </c>
       <c r="L109" s="9">
-        <f>J109*K109</f>
+        <f t="shared" si="14"/>
         <v>16.237500000000001</v>
       </c>
       <c r="M109" s="9">
-        <f>J109-L109</f>
+        <f t="shared" si="15"/>
         <v>308.51249999999999</v>
       </c>
     </row>
@@ -6120,7 +6120,7 @@
         <v>42499</v>
       </c>
       <c r="G110" s="8">
-        <f>F110-E110</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="H110" s="2">
@@ -6130,18 +6130,18 @@
         <v>37.99</v>
       </c>
       <c r="J110" s="9">
-        <f>H110*I110</f>
+        <f t="shared" si="13"/>
         <v>721.81000000000006</v>
       </c>
       <c r="K110" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L110" s="9">
-        <f>J110*K110</f>
+        <f t="shared" si="14"/>
         <v>50.526700000000012</v>
       </c>
       <c r="M110" s="9">
-        <f>J110-L110</f>
+        <f t="shared" si="15"/>
         <v>671.28330000000005</v>
       </c>
     </row>
@@ -6165,7 +6165,7 @@
         <v>42500</v>
       </c>
       <c r="G111" s="8">
-        <f>F111-E111</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H111" s="2">
@@ -6175,18 +6175,18 @@
         <v>32.99</v>
       </c>
       <c r="J111" s="9">
-        <f>H111*I111</f>
+        <f t="shared" si="13"/>
         <v>692.79000000000008</v>
       </c>
       <c r="K111" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L111" s="9">
-        <f>J111*K111</f>
+        <f t="shared" si="14"/>
         <v>51.959250000000004</v>
       </c>
       <c r="M111" s="9">
-        <f>J111-L111</f>
+        <f t="shared" si="15"/>
         <v>640.83075000000008</v>
       </c>
     </row>
@@ -6210,7 +6210,7 @@
         <v>42495</v>
       </c>
       <c r="G112" s="8">
-        <f>F112-E112</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H112" s="2">
@@ -6220,18 +6220,18 @@
         <v>32.99</v>
       </c>
       <c r="J112" s="9">
-        <f>H112*I112</f>
+        <f t="shared" si="13"/>
         <v>725.78000000000009</v>
       </c>
       <c r="K112" s="10">
         <v>0.05</v>
       </c>
       <c r="L112" s="9">
-        <f>J112*K112</f>
+        <f t="shared" si="14"/>
         <v>36.289000000000009</v>
       </c>
       <c r="M112" s="9">
-        <f>J112-L112</f>
+        <f t="shared" si="15"/>
         <v>689.4910000000001</v>
       </c>
     </row>
@@ -6255,7 +6255,7 @@
         <v>42498</v>
       </c>
       <c r="G113" s="8">
-        <f>F113-E113</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="H113" s="2">
@@ -6265,18 +6265,18 @@
         <v>32.99</v>
       </c>
       <c r="J113" s="9">
-        <f>H113*I113</f>
+        <f t="shared" si="13"/>
         <v>692.79000000000008</v>
       </c>
       <c r="K113" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L113" s="9">
-        <f>J113*K113</f>
+        <f t="shared" si="14"/>
         <v>45.031350000000003</v>
       </c>
       <c r="M113" s="9">
-        <f>J113-L113</f>
+        <f t="shared" si="15"/>
         <v>647.7586500000001</v>
       </c>
     </row>
@@ -6300,7 +6300,7 @@
         <v>42516</v>
       </c>
       <c r="G114" s="8">
-        <f>F114-E114</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H114" s="2">
@@ -6310,18 +6310,18 @@
         <v>32.99</v>
       </c>
       <c r="J114" s="9">
-        <f>H114*I114</f>
+        <f t="shared" si="13"/>
         <v>395.88</v>
       </c>
       <c r="K114" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L114" s="9">
-        <f>J114*K114</f>
+        <f t="shared" si="14"/>
         <v>27.711600000000001</v>
       </c>
       <c r="M114" s="9">
-        <f>J114-L114</f>
+        <f t="shared" si="15"/>
         <v>368.16840000000002</v>
       </c>
     </row>
@@ -6345,7 +6345,7 @@
         <v>42525</v>
       </c>
       <c r="G115" s="8">
-        <f>F115-E115</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H115" s="2">
@@ -6355,18 +6355,18 @@
         <v>25.99</v>
       </c>
       <c r="J115" s="9">
-        <f>H115*I115</f>
+        <f t="shared" si="13"/>
         <v>623.76</v>
       </c>
       <c r="K115" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L115" s="9">
-        <f>J115*K115</f>
+        <f t="shared" si="14"/>
         <v>43.663200000000003</v>
       </c>
       <c r="M115" s="9">
-        <f>J115-L115</f>
+        <f t="shared" si="15"/>
         <v>580.09680000000003</v>
       </c>
     </row>
@@ -6390,7 +6390,7 @@
         <v>42520</v>
       </c>
       <c r="G116" s="8">
-        <f>F116-E116</f>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="H116" s="2">
@@ -6400,18 +6400,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J116" s="9">
-        <f>H116*I116</f>
+        <f t="shared" si="13"/>
         <v>373.78</v>
       </c>
       <c r="K116" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L116" s="9">
-        <f>J116*K116</f>
+        <f t="shared" si="14"/>
         <v>26.1646</v>
       </c>
       <c r="M116" s="9">
-        <f>J116-L116</f>
+        <f t="shared" si="15"/>
         <v>347.61539999999997</v>
       </c>
     </row>
@@ -6435,7 +6435,7 @@
         <v>42532</v>
       </c>
       <c r="G117" s="8">
-        <f>F117-E117</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H117" s="2">
@@ -6445,18 +6445,18 @@
         <v>32.99</v>
       </c>
       <c r="J117" s="9">
-        <f>H117*I117</f>
+        <f t="shared" si="13"/>
         <v>725.78000000000009</v>
       </c>
       <c r="K117" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L117" s="9">
-        <f>J117*K117</f>
+        <f t="shared" si="14"/>
         <v>54.433500000000002</v>
       </c>
       <c r="M117" s="9">
-        <f>J117-L117</f>
+        <f t="shared" si="15"/>
         <v>671.34650000000011</v>
       </c>
     </row>
@@ -6480,7 +6480,7 @@
         <v>42532</v>
       </c>
       <c r="G118" s="8">
-        <f>F118-E118</f>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="H118" s="2">
@@ -6490,18 +6490,18 @@
         <v>23.99</v>
       </c>
       <c r="J118" s="9">
-        <f>H118*I118</f>
+        <f t="shared" si="13"/>
         <v>623.74</v>
       </c>
       <c r="K118" s="10">
         <v>0.05</v>
       </c>
       <c r="L118" s="9">
-        <f>J118*K118</f>
+        <f t="shared" si="14"/>
         <v>31.187000000000001</v>
       </c>
       <c r="M118" s="9">
-        <f>J118-L118</f>
+        <f t="shared" si="15"/>
         <v>592.553</v>
       </c>
     </row>
@@ -6525,7 +6525,7 @@
         <v>42528</v>
       </c>
       <c r="G119" s="8">
-        <f>F119-E119</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="H119" s="2">
@@ -6535,18 +6535,18 @@
         <v>9.99</v>
       </c>
       <c r="J119" s="9">
-        <f>H119*I119</f>
+        <f t="shared" si="13"/>
         <v>249.75</v>
       </c>
       <c r="K119" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L119" s="9">
-        <f>J119*K119</f>
+        <f t="shared" si="14"/>
         <v>17.482500000000002</v>
       </c>
       <c r="M119" s="9">
-        <f>J119-L119</f>
+        <f t="shared" si="15"/>
         <v>232.26749999999998</v>
       </c>
     </row>
@@ -6570,7 +6570,7 @@
         <v>42536</v>
       </c>
       <c r="G120" s="8">
-        <f>F120-E120</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H120" s="2">
@@ -6580,18 +6580,18 @@
         <v>25.99</v>
       </c>
       <c r="J120" s="9">
-        <f>H120*I120</f>
+        <f t="shared" si="13"/>
         <v>441.83</v>
       </c>
       <c r="K120" s="10">
         <v>0.05</v>
       </c>
       <c r="L120" s="9">
-        <f>J120*K120</f>
+        <f t="shared" si="14"/>
         <v>22.0915</v>
       </c>
       <c r="M120" s="9">
-        <f>J120-L120</f>
+        <f t="shared" si="15"/>
         <v>419.73849999999999</v>
       </c>
     </row>
@@ -6615,7 +6615,7 @@
         <v>42532</v>
       </c>
       <c r="G121" s="8">
-        <f>F121-E121</f>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="H121" s="2">
@@ -6625,18 +6625,18 @@
         <v>23.99</v>
       </c>
       <c r="J121" s="9">
-        <f>H121*I121</f>
+        <f t="shared" si="13"/>
         <v>551.77</v>
       </c>
       <c r="K121" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L121" s="9">
-        <f>J121*K121</f>
+        <f t="shared" si="14"/>
         <v>35.865049999999997</v>
       </c>
       <c r="M121" s="9">
-        <f>J121-L121</f>
+        <f t="shared" si="15"/>
         <v>515.90494999999999</v>
       </c>
     </row>
@@ -6660,7 +6660,7 @@
         <v>42531</v>
       </c>
       <c r="G122" s="8">
-        <f>F122-E122</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H122" s="2">
@@ -6670,18 +6670,18 @@
         <v>49.99</v>
       </c>
       <c r="J122" s="9">
-        <f>H122*I122</f>
+        <f t="shared" si="13"/>
         <v>799.84</v>
       </c>
       <c r="K122" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L122" s="9">
-        <f>J122*K122</f>
+        <f t="shared" si="14"/>
         <v>55.988800000000005</v>
       </c>
       <c r="M122" s="9">
-        <f>J122-L122</f>
+        <f t="shared" si="15"/>
         <v>743.85120000000006</v>
       </c>
     </row>
@@ -6705,7 +6705,7 @@
         <v>42548</v>
       </c>
       <c r="G123" s="8">
-        <f>F123-E123</f>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
       <c r="H123" s="2">
@@ -6715,18 +6715,18 @@
         <v>9.99</v>
       </c>
       <c r="J123" s="9">
-        <f>H123*I123</f>
+        <f t="shared" si="13"/>
         <v>219.78</v>
       </c>
       <c r="K123" s="10">
         <v>0.06</v>
       </c>
       <c r="L123" s="9">
-        <f>J123*K123</f>
+        <f t="shared" si="14"/>
         <v>13.1868</v>
       </c>
       <c r="M123" s="9">
-        <f>J123-L123</f>
+        <f t="shared" si="15"/>
         <v>206.5932</v>
       </c>
     </row>
@@ -6750,7 +6750,7 @@
         <v>42544</v>
       </c>
       <c r="G124" s="8">
-        <f>F124-E124</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="H124" s="2">
@@ -6760,18 +6760,18 @@
         <v>23.99</v>
       </c>
       <c r="J124" s="9">
-        <f>H124*I124</f>
+        <f t="shared" si="13"/>
         <v>623.74</v>
       </c>
       <c r="K124" s="10">
         <v>0.05</v>
       </c>
       <c r="L124" s="9">
-        <f>J124*K124</f>
+        <f t="shared" si="14"/>
         <v>31.187000000000001</v>
       </c>
       <c r="M124" s="9">
-        <f>J124-L124</f>
+        <f t="shared" si="15"/>
         <v>592.553</v>
       </c>
     </row>
@@ -6795,7 +6795,7 @@
         <v>42544</v>
       </c>
       <c r="G125" s="8">
-        <f>F125-E125</f>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="H125" s="2">
@@ -6805,18 +6805,18 @@
         <v>32.99</v>
       </c>
       <c r="J125" s="9">
-        <f>H125*I125</f>
+        <f t="shared" si="13"/>
         <v>791.76</v>
       </c>
       <c r="K125" s="10">
         <v>0.06</v>
       </c>
       <c r="L125" s="9">
-        <f>J125*K125</f>
+        <f t="shared" si="14"/>
         <v>47.505600000000001</v>
       </c>
       <c r="M125" s="9">
-        <f>J125-L125</f>
+        <f t="shared" si="15"/>
         <v>744.25440000000003</v>
       </c>
     </row>
@@ -6840,7 +6840,7 @@
         <v>42377</v>
       </c>
       <c r="G126" s="8">
-        <f>F126-E126</f>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="H126" s="2">
@@ -6850,18 +6850,18 @@
         <v>37.99</v>
       </c>
       <c r="J126" s="9">
-        <f>H126*I126</f>
+        <f t="shared" si="13"/>
         <v>911.76</v>
       </c>
       <c r="K126" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L126" s="9">
-        <f>J126*K126</f>
+        <f t="shared" si="14"/>
         <v>59.264400000000002</v>
       </c>
       <c r="M126" s="9">
-        <f>J126-L126</f>
+        <f t="shared" si="15"/>
         <v>852.49559999999997</v>
       </c>
     </row>
@@ -6885,7 +6885,7 @@
         <v>42381</v>
       </c>
       <c r="G127" s="8">
-        <f>F127-E127</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H127" s="2">
@@ -6895,18 +6895,18 @@
         <v>21.99</v>
       </c>
       <c r="J127" s="9">
-        <f>H127*I127</f>
+        <f t="shared" si="13"/>
         <v>461.78999999999996</v>
       </c>
       <c r="K127" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L127" s="9">
-        <f>J127*K127</f>
+        <f t="shared" si="14"/>
         <v>34.634249999999994</v>
       </c>
       <c r="M127" s="9">
-        <f>J127-L127</f>
+        <f t="shared" si="15"/>
         <v>427.15574999999995</v>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
         <v>42395</v>
       </c>
       <c r="G128" s="8">
-        <f>F128-E128</f>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="H128" s="2">
@@ -6940,18 +6940,18 @@
         <v>12.99</v>
       </c>
       <c r="J128" s="9">
-        <f>H128*I128</f>
+        <f t="shared" si="13"/>
         <v>311.76</v>
       </c>
       <c r="K128" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L128" s="9">
-        <f>J128*K128</f>
+        <f t="shared" si="14"/>
         <v>21.8232</v>
       </c>
       <c r="M128" s="9">
-        <f>J128-L128</f>
+        <f t="shared" si="15"/>
         <v>289.93680000000001</v>
       </c>
     </row>
@@ -6975,7 +6975,7 @@
         <v>42407</v>
       </c>
       <c r="G129" s="8">
-        <f>F129-E129</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H129" s="2">
@@ -6985,18 +6985,18 @@
         <v>49.99</v>
       </c>
       <c r="J129" s="9">
-        <f>H129*I129</f>
+        <f t="shared" si="13"/>
         <v>849.83</v>
       </c>
       <c r="K129" s="10">
         <v>0.06</v>
       </c>
       <c r="L129" s="9">
-        <f>J129*K129</f>
+        <f t="shared" si="14"/>
         <v>50.989800000000002</v>
       </c>
       <c r="M129" s="9">
-        <f>J129-L129</f>
+        <f t="shared" si="15"/>
         <v>798.8402000000001</v>
       </c>
     </row>
@@ -7020,7 +7020,7 @@
         <v>42419</v>
       </c>
       <c r="G130" s="8">
-        <f>F130-E130</f>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="H130" s="2">
@@ -7030,18 +7030,18 @@
         <v>16.989999999999998</v>
       </c>
       <c r="J130" s="9">
-        <f>H130*I130</f>
+        <f t="shared" si="13"/>
         <v>305.82</v>
       </c>
       <c r="K130" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L130" s="9">
-        <f>J130*K130</f>
+        <f t="shared" si="14"/>
         <v>19.878299999999999</v>
       </c>
       <c r="M130" s="9">
-        <f>J130-L130</f>
+        <f t="shared" si="15"/>
         <v>285.94169999999997</v>
       </c>
     </row>
@@ -7065,7 +7065,7 @@
         <v>42438</v>
       </c>
       <c r="G131" s="8">
-        <f>F131-E131</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="H131" s="2">
@@ -7075,18 +7075,18 @@
         <v>12.99</v>
       </c>
       <c r="J131" s="9">
-        <f>H131*I131</f>
+        <f t="shared" si="13"/>
         <v>246.81</v>
       </c>
       <c r="K131" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L131" s="9">
-        <f>J131*K131</f>
+        <f t="shared" si="14"/>
         <v>16.042650000000002</v>
       </c>
       <c r="M131" s="9">
-        <f>J131-L131</f>
+        <f t="shared" si="15"/>
         <v>230.76734999999999</v>
       </c>
     </row>
@@ -7110,7 +7110,7 @@
         <v>42449</v>
       </c>
       <c r="G132" s="8">
-        <f>F132-E132</f>
+        <f t="shared" ref="G132:G142" si="16">F132-E132</f>
         <v>15</v>
       </c>
       <c r="H132" s="2">
@@ -7120,18 +7120,18 @@
         <v>21.99</v>
       </c>
       <c r="J132" s="9">
-        <f>H132*I132</f>
+        <f t="shared" ref="J132:J142" si="17">H132*I132</f>
         <v>263.88</v>
       </c>
       <c r="K132" s="10">
         <v>0.05</v>
       </c>
       <c r="L132" s="9">
-        <f>J132*K132</f>
+        <f t="shared" ref="L132:L142" si="18">J132*K132</f>
         <v>13.194000000000001</v>
       </c>
       <c r="M132" s="9">
-        <f>J132-L132</f>
+        <f t="shared" ref="M132:M142" si="19">J132-L132</f>
         <v>250.68600000000001</v>
       </c>
     </row>
@@ -7155,7 +7155,7 @@
         <v>42451</v>
       </c>
       <c r="G133" s="8">
-        <f>F133-E133</f>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="H133" s="2">
@@ -7165,18 +7165,18 @@
         <v>12.99</v>
       </c>
       <c r="J133" s="9">
-        <f>H133*I133</f>
+        <f t="shared" si="17"/>
         <v>272.79000000000002</v>
       </c>
       <c r="K133" s="10">
         <v>0.05</v>
       </c>
       <c r="L133" s="9">
-        <f>J133*K133</f>
+        <f t="shared" si="18"/>
         <v>13.639500000000002</v>
       </c>
       <c r="M133" s="9">
-        <f>J133-L133</f>
+        <f t="shared" si="19"/>
         <v>259.15050000000002</v>
       </c>
     </row>
@@ -7200,7 +7200,7 @@
         <v>42454</v>
       </c>
       <c r="G134" s="8">
-        <f>F134-E134</f>
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="H134" s="2">
@@ -7210,18 +7210,18 @@
         <v>37.99</v>
       </c>
       <c r="J134" s="9">
-        <f>H134*I134</f>
+        <f t="shared" si="17"/>
         <v>949.75</v>
       </c>
       <c r="K134" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L134" s="9">
-        <f>J134*K134</f>
+        <f t="shared" si="18"/>
         <v>71.231250000000003</v>
       </c>
       <c r="M134" s="9">
-        <f>J134-L134</f>
+        <f t="shared" si="19"/>
         <v>878.51874999999995</v>
       </c>
     </row>
@@ -7245,7 +7245,7 @@
         <v>42462</v>
       </c>
       <c r="G135" s="8">
-        <f>F135-E135</f>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="H135" s="2">
@@ -7255,18 +7255,18 @@
         <v>42.99</v>
       </c>
       <c r="J135" s="9">
-        <f>H135*I135</f>
+        <f t="shared" si="17"/>
         <v>773.82</v>
       </c>
       <c r="K135" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="L135" s="9">
-        <f>J135*K135</f>
+        <f t="shared" si="18"/>
         <v>58.036500000000004</v>
       </c>
       <c r="M135" s="9">
-        <f>J135-L135</f>
+        <f t="shared" si="19"/>
         <v>715.7835</v>
       </c>
     </row>
@@ -7290,7 +7290,7 @@
         <v>42456</v>
       </c>
       <c r="G136" s="8">
-        <f>F136-E136</f>
+        <f t="shared" si="16"/>
         <v>6</v>
       </c>
       <c r="H136" s="2">
@@ -7300,18 +7300,18 @@
         <v>32.99</v>
       </c>
       <c r="J136" s="9">
-        <f>H136*I136</f>
+        <f t="shared" si="17"/>
         <v>659.80000000000007</v>
       </c>
       <c r="K136" s="10">
         <v>0.06</v>
       </c>
       <c r="L136" s="9">
-        <f>J136*K136</f>
+        <f t="shared" si="18"/>
         <v>39.588000000000001</v>
       </c>
       <c r="M136" s="9">
-        <f>J136-L136</f>
+        <f t="shared" si="19"/>
         <v>620.2120000000001</v>
       </c>
     </row>
@@ -7335,7 +7335,7 @@
         <v>42487</v>
       </c>
       <c r="G137" s="8">
-        <f>F137-E137</f>
+        <f t="shared" si="16"/>
         <v>13</v>
       </c>
       <c r="H137" s="2">
@@ -7345,18 +7345,18 @@
         <v>32.99</v>
       </c>
       <c r="J137" s="9">
-        <f>H137*I137</f>
+        <f t="shared" si="17"/>
         <v>857.74</v>
       </c>
       <c r="K137" s="10">
         <v>0.05</v>
       </c>
       <c r="L137" s="9">
-        <f>J137*K137</f>
+        <f t="shared" si="18"/>
         <v>42.887</v>
       </c>
       <c r="M137" s="9">
-        <f>J137-L137</f>
+        <f t="shared" si="19"/>
         <v>814.85300000000007</v>
       </c>
     </row>
@@ -7380,7 +7380,7 @@
         <v>42520</v>
       </c>
       <c r="G138" s="8">
-        <f>F138-E138</f>
+        <f t="shared" si="16"/>
         <v>14</v>
       </c>
       <c r="H138" s="2">
@@ -7390,18 +7390,18 @@
         <v>23.99</v>
       </c>
       <c r="J138" s="9">
-        <f>H138*I138</f>
+        <f t="shared" si="17"/>
         <v>431.82</v>
       </c>
       <c r="K138" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L138" s="9">
-        <f>J138*K138</f>
+        <f t="shared" si="18"/>
         <v>30.227400000000003</v>
       </c>
       <c r="M138" s="9">
-        <f>J138-L138</f>
+        <f t="shared" si="19"/>
         <v>401.5926</v>
       </c>
     </row>
@@ -7425,7 +7425,7 @@
         <v>42522</v>
       </c>
       <c r="G139" s="8">
-        <f>F139-E139</f>
+        <f t="shared" si="16"/>
         <v>5</v>
       </c>
       <c r="H139" s="2">
@@ -7435,18 +7435,18 @@
         <v>32.99</v>
       </c>
       <c r="J139" s="9">
-        <f>H139*I139</f>
+        <f t="shared" si="17"/>
         <v>692.79000000000008</v>
       </c>
       <c r="K139" s="10">
         <v>0.05</v>
       </c>
       <c r="L139" s="9">
-        <f>J139*K139</f>
+        <f t="shared" si="18"/>
         <v>34.639500000000005</v>
       </c>
       <c r="M139" s="9">
-        <f>J139-L139</f>
+        <f t="shared" si="19"/>
         <v>658.15050000000008</v>
       </c>
     </row>
@@ -7470,7 +7470,7 @@
         <v>42532</v>
       </c>
       <c r="G140" s="8">
-        <f>F140-E140</f>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="H140" s="2">
@@ -7480,18 +7480,18 @@
         <v>32.99</v>
       </c>
       <c r="J140" s="9">
-        <f>H140*I140</f>
+        <f t="shared" si="17"/>
         <v>494.85</v>
       </c>
       <c r="K140" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L140" s="9">
-        <f>J140*K140</f>
+        <f t="shared" si="18"/>
         <v>32.16525</v>
       </c>
       <c r="M140" s="9">
-        <f>J140-L140</f>
+        <f t="shared" si="19"/>
         <v>462.68475000000001</v>
       </c>
     </row>
@@ -7515,7 +7515,7 @@
         <v>42527</v>
       </c>
       <c r="G141" s="8">
-        <f>F141-E141</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="H141" s="2">
@@ -7525,18 +7525,18 @@
         <v>12.99</v>
       </c>
       <c r="J141" s="9">
-        <f>H141*I141</f>
+        <f t="shared" si="17"/>
         <v>272.79000000000002</v>
       </c>
       <c r="K141" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="L141" s="9">
-        <f>J141*K141</f>
+        <f t="shared" si="18"/>
         <v>17.731350000000003</v>
       </c>
       <c r="M141" s="9">
-        <f>J141-L141</f>
+        <f t="shared" si="19"/>
         <v>255.05865000000003</v>
       </c>
     </row>
@@ -7560,7 +7560,7 @@
         <v>42541</v>
       </c>
       <c r="G142" s="8">
-        <f>F142-E142</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="H142" s="2">
@@ -7570,18 +7570,18 @@
         <v>23.99</v>
       </c>
       <c r="J142" s="9">
-        <f>H142*I142</f>
+        <f t="shared" si="17"/>
         <v>359.84999999999997</v>
       </c>
       <c r="K142" s="10">
         <v>0.06</v>
       </c>
       <c r="L142" s="9">
-        <f>J142*K142</f>
+        <f t="shared" si="18"/>
         <v>21.590999999999998</v>
       </c>
       <c r="M142" s="9">
-        <f>J142-L142</f>
+        <f t="shared" si="19"/>
         <v>338.25899999999996</v>
       </c>
     </row>
@@ -12525,7 +12525,8 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;P of &amp;N</oddHeader>
+    <oddHeader xml:space="preserve">&amp;L&amp;P of &amp;N&amp;R&amp;D
+</oddHeader>
   </headerFooter>
   <rowBreaks count="4" manualBreakCount="4">
     <brk id="23" max="16383" man="1"/>

</xml_diff>